<commit_message>
update 04 - 12
</commit_message>
<xml_diff>
--- a/MakeMoney/Thong_Ke/xls/Cau_T2.xlsx
+++ b/MakeMoney/Thong_Ke/xls/Cau_T2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="10" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="507" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="10" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="499" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="CK" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="55">
   <si>
     <t>Cau so 10</t>
   </si>
@@ -530,9 +530,9 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.89803921568628"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="54.7725490196078"/>
-    <col collapsed="false" hidden="false" max="257" min="3" style="0" width="8.89803921568628"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.94509803921569"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.043137254902"/>
+    <col collapsed="false" hidden="false" max="257" min="3" style="0" width="8.94509803921569"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
@@ -687,41 +687,41 @@
   <dimension ref="A1:AF29"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A10" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <selection activeCell="D29" activeCellId="0" pane="topLeft" sqref="D29"/>
+      <selection activeCell="E29" activeCellId="0" pane="topLeft" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9647058823529"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="4.52941176470588"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="3.95294117647059"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="4.08627450980392"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="4.69411764705882"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="5" width="4.52941176470588"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="4.24313725490196"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="5" width="4.83137254901961"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="5" width="4.69411764705882"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="5" width="4.38823529411765"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="5" width="4.9843137254902"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="5" width="4.52941176470588"/>
-    <col collapsed="false" hidden="false" max="14" min="13" style="5" width="5.4156862745098"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="5" width="4.83137254901961"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="5" width="4.52941176470588"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="5" width="4.83137254901961"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="5" width="4.52941176470588"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="5" width="4.69411764705882"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="5" width="5.70588235294118"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="5" width="5.4156862745098"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="5" width="4.9843137254902"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="5" width="5.4156862745098"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="5" width="5.27450980392157"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="5" width="4.52941176470588"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="5" width="5.12941176470588"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="5" width="4.24313725490196"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="5" width="4.52941176470588"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="5" width="3.95294117647059"/>
-    <col collapsed="false" hidden="false" max="31" min="30" style="5" width="4.69411764705882"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="5" width="5.4156862745098"/>
-    <col collapsed="false" hidden="false" max="257" min="33" style="0" width="8.89803921568628"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.043137254902"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="4.54901960784314"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="3.96862745098039"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="4.10588235294118"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="4.72156862745098"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="5" width="4.54901960784314"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="4.27058823529412"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="5" width="4.85490196078431"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="5" width="4.72156862745098"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="5" width="4.41176470588235"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="5" width="5.01176470588235"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="5" width="4.54901960784314"/>
+    <col collapsed="false" hidden="false" max="14" min="13" style="5" width="5.44313725490196"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="5" width="4.85490196078431"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="5" width="4.54901960784314"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="5" width="4.85490196078431"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="5" width="4.54901960784314"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="5" width="4.72156862745098"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="5" width="5.73333333333333"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="5" width="5.44313725490196"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="5" width="5.01176470588235"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="5" width="5.44313725490196"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="5" width="5.29803921568627"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="5" width="4.54901960784314"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="5" width="5.15686274509804"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="5" width="4.27058823529412"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="5" width="4.54901960784314"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="5" width="3.96862745098039"/>
+    <col collapsed="false" hidden="false" max="31" min="30" style="5" width="4.72156862745098"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="5" width="5.44313725490196"/>
+    <col collapsed="false" hidden="false" max="257" min="33" style="0" width="8.94509803921569"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
@@ -1583,6 +1583,9 @@
       <c r="D28" s="5" t="n">
         <v>50</v>
       </c>
+      <c r="E28" s="5" t="n">
+        <v>81</v>
+      </c>
       <c r="S28" s="27"/>
       <c r="T28" s="27"/>
     </row>
@@ -1590,10 +1593,12 @@
       <c r="A29" s="25"/>
       <c r="B29" s="7"/>
       <c r="C29" s="10"/>
-      <c r="D29" s="10" t="s">
+      <c r="D29" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E29" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="E29" s="10"/>
       <c r="F29" s="10"/>
       <c r="G29" s="7"/>
       <c r="H29" s="10"/>
@@ -1641,40 +1646,40 @@
   <dimension ref="A1:AF65"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A43" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <selection activeCell="D65" activeCellId="0" pane="topLeft" sqref="D65"/>
+      <selection activeCell="E65" activeCellId="0" pane="topLeft" sqref="E65"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9647058823529"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="4.38823529411765"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="4.52941176470588"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="4.08627450980392"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="4.69411764705882"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="5" width="4.38823529411765"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="4.24313725490196"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="5" width="4.9843137254902"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="5" width="4.69411764705882"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="5" width="4.52941176470588"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="5" width="4.9843137254902"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="5" width="4.52941176470588"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="5" width="4.69411764705882"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="5" width="5.4156862745098"/>
-    <col collapsed="false" hidden="false" max="16" min="15" style="5" width="4.69411764705882"/>
-    <col collapsed="false" hidden="false" max="18" min="17" style="5" width="4.9843137254902"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="5" width="4.69411764705882"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="5" width="5.70588235294118"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="5" width="5.4156862745098"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="5" width="5.56078431372549"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="5" width="5.4156862745098"/>
-    <col collapsed="false" hidden="false" max="25" min="24" style="5" width="4.9843137254902"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="5" width="4.38823529411765"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="5" width="4.24313725490196"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="5" width="4.69411764705882"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="5" width="3.95294117647059"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="5" width="4.08627450980392"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="5" width="4.52941176470588"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="5" width="3.8"/>
-    <col collapsed="false" hidden="false" max="257" min="33" style="0" width="8.89803921568628"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.043137254902"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="4.41176470588235"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="4.54901960784314"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="4.10588235294118"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="4.72156862745098"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="5" width="4.41176470588235"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="4.27058823529412"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="5" width="5.01176470588235"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="5" width="4.72156862745098"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="5" width="4.54901960784314"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="5" width="5.01176470588235"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="5" width="4.54901960784314"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="5" width="4.72156862745098"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="5" width="5.44313725490196"/>
+    <col collapsed="false" hidden="false" max="16" min="15" style="5" width="4.72156862745098"/>
+    <col collapsed="false" hidden="false" max="18" min="17" style="5" width="5.01176470588235"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="5" width="4.72156862745098"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="5" width="5.73333333333333"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="5" width="5.44313725490196"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="5" width="5.58823529411765"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="5" width="5.44313725490196"/>
+    <col collapsed="false" hidden="false" max="25" min="24" style="5" width="5.01176470588235"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="5" width="4.41176470588235"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="5" width="4.27058823529412"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="5" width="4.72156862745098"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="5" width="3.96862745098039"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="5" width="4.10588235294118"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="5" width="4.54901960784314"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="5" width="3.8156862745098"/>
+    <col collapsed="false" hidden="false" max="257" min="33" style="0" width="8.94509803921569"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
@@ -3516,10 +3521,10 @@
       <c r="A65" s="25"/>
       <c r="B65" s="7"/>
       <c r="C65" s="10"/>
-      <c r="D65" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="E65" s="10"/>
+      <c r="D65" s="10"/>
+      <c r="E65" s="10" t="n">
+        <v>0</v>
+      </c>
       <c r="F65" s="10"/>
       <c r="G65" s="7"/>
       <c r="H65" s="10"/>
@@ -3571,39 +3576,39 @@
   <dimension ref="A1:AF69"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A58" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <selection activeCell="D69" activeCellId="0" pane="topLeft" sqref="D69"/>
+      <selection activeCell="E69" activeCellId="0" pane="topLeft" sqref="E69"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9647058823529"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="5.27450980392157"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="6.14901960784314"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="5.4156862745098"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="5" width="5.56078431372549"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="5.27450980392157"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="5" width="5.56078431372549"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="5" width="5.70588235294118"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="5" width="5.56078431372549"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="5" width="4.9843137254902"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="5" width="5.56078431372549"/>
-    <col collapsed="false" hidden="false" max="16" min="13" style="5" width="5.4156862745098"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="5" width="5.56078431372549"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="5" width="4.69411764705882"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="5" width="4.9843137254902"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="5" width="5.84313725490196"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="5" width="5.70588235294118"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="5" width="5.34509803921569"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="5" width="5.49803921568627"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="5" width="5.1921568627451"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="5" width="5.65098039215686"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="5" width="5.1921568627451"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="5" width="5.84313725490196"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="5" width="4.69411764705882"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="5" width="4.38823529411765"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="5" width="4.24313725490196"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="5" width="4.69411764705882"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="5" width="4.83137254901961"/>
-    <col collapsed="false" hidden="false" max="257" min="33" style="0" width="8.89803921568628"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.043137254902"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="5.29803921568627"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="6.17647058823529"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="5.44313725490196"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="5" width="5.58823529411765"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="5.29803921568627"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="5" width="5.58823529411765"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="5" width="5.73333333333333"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="5" width="5.58823529411765"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="5" width="5.01176470588235"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="5" width="5.58823529411765"/>
+    <col collapsed="false" hidden="false" max="16" min="13" style="5" width="5.44313725490196"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="5" width="5.58823529411765"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="5" width="4.72156862745098"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="5" width="5.01176470588235"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="5" width="5.87058823529412"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="5" width="5.73333333333333"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="5" width="5.37254901960784"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="5" width="5.52549019607843"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="5" width="5.21960784313726"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="5" width="5.67843137254902"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="5" width="5.21960784313726"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="5" width="5.87058823529412"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="5" width="4.72156862745098"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="5" width="4.41176470588235"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="5" width="4.27058823529412"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="5" width="4.72156862745098"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="5" width="4.85490196078431"/>
+    <col collapsed="false" hidden="false" max="257" min="33" style="0" width="8.94509803921569"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
@@ -5366,7 +5371,7 @@
         <v>42</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="66">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.25" outlineLevel="0" r="66">
       <c r="A66" s="25"/>
       <c r="B66" s="7" t="n">
         <v>2</v>
@@ -5420,10 +5425,10 @@
       <c r="AA66" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="AB66" s="7"/>
-      <c r="AC66" s="7"/>
-      <c r="AD66" s="7"/>
-      <c r="AE66" s="7"/>
+      <c r="AB66" s="11"/>
+      <c r="AC66" s="11"/>
+      <c r="AD66" s="11"/>
+      <c r="AE66" s="11"/>
       <c r="AF66" s="19"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="17.6" outlineLevel="0" r="68">
@@ -5439,17 +5444,24 @@
       <c r="D68" s="5" t="s">
         <v>44</v>
       </c>
+      <c r="E68" s="5" t="n">
+        <v>19</v>
+      </c>
       <c r="S68" s="27"/>
       <c r="T68" s="27"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.25" outlineLevel="0" r="69">
       <c r="A69" s="25"/>
-      <c r="B69" s="7"/>
-      <c r="C69" s="10"/>
-      <c r="D69" s="10" t="s">
+      <c r="B69" s="11"/>
+      <c r="C69" s="13" t="n">
+        <v>6</v>
+      </c>
+      <c r="D69" s="13" t="n">
+        <v>7</v>
+      </c>
+      <c r="E69" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="E69" s="10"/>
       <c r="F69" s="10"/>
       <c r="G69" s="7"/>
       <c r="H69" s="10"/>
@@ -5501,39 +5513,39 @@
   <dimension ref="A1:AF30"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <selection activeCell="D30" activeCellId="0" pane="topLeft" sqref="D30"/>
+      <selection activeCell="E30" activeCellId="0" pane="topLeft" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.9176470588235"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="4.83137254901961"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="5" width="5.56078431372549"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="6.31372549019608"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="5" width="5.27450980392157"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="5" width="4.9843137254902"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="5" width="4.69411764705882"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="5" width="5.27450980392157"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="5" width="4.9843137254902"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="5" width="4.52941176470588"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="5" width="4.83137254901961"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="5" width="4.69411764705882"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="5" width="5.70588235294118"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="5" width="5.27450980392157"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="5" width="5.56078431372549"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="5" width="5.70588235294118"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="5" width="6.14901960784314"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="5" width="5.70588235294118"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="5" width="5.4156862745098"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="5" width="5.56078431372549"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="5" width="5.12941176470588"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="5" width="4.9843137254902"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="5" width="5.12941176470588"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="5" width="5.27450980392157"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="5" width="4.83137254901961"/>
-    <col collapsed="false" hidden="false" max="30" min="28" style="5" width="5.12941176470588"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="5" width="4.38823529411765"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="5" width="5.70588235294118"/>
-    <col collapsed="false" hidden="false" max="257" min="33" style="0" width="8.89803921568628"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.9921568627451"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="4.85490196078431"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="5" width="5.58823529411765"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="6.34117647058824"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="5" width="5.29803921568627"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="5" width="5.01176470588235"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="5" width="4.72156862745098"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="5" width="5.29803921568627"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="5" width="5.01176470588235"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="5" width="4.54901960784314"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="5" width="4.85490196078431"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="5" width="4.72156862745098"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="5" width="5.73333333333333"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="5" width="5.29803921568627"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="5" width="5.58823529411765"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="5" width="5.73333333333333"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="5" width="6.17647058823529"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="5" width="5.73333333333333"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="5" width="5.44313725490196"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="5" width="5.58823529411765"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="5" width="5.15686274509804"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="5" width="5.01176470588235"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="5" width="5.15686274509804"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="5" width="5.29803921568627"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="5" width="4.85490196078431"/>
+    <col collapsed="false" hidden="false" max="30" min="28" style="5" width="5.15686274509804"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="5" width="4.41176470588235"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="5" width="5.73333333333333"/>
+    <col collapsed="false" hidden="false" max="257" min="33" style="0" width="8.94509803921569"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
@@ -6415,6 +6427,9 @@
       <c r="D29" s="5" t="n">
         <v>28</v>
       </c>
+      <c r="E29" s="5" t="n">
+        <v>24</v>
+      </c>
       <c r="S29" s="27"/>
       <c r="T29" s="27"/>
     </row>
@@ -6426,10 +6441,10 @@
       <c r="C30" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="D30" s="10" t="s">
+      <c r="D30" s="10"/>
+      <c r="E30" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="E30" s="10"/>
       <c r="F30" s="10"/>
       <c r="G30" s="7"/>
       <c r="H30" s="10"/>
@@ -6477,40 +6492,40 @@
   <dimension ref="A1:AF74"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A58" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <selection activeCell="D74" activeCellId="0" pane="topLeft" sqref="D74"/>
+      <selection activeCell="E74" activeCellId="0" pane="topLeft" sqref="E74"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9647058823529"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="4.9843137254902"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="4.69411764705882"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="5.4156862745098"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="5.12941176470588"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="5" width="4.38823529411765"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="4.24313725490196"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="5" width="4.69411764705882"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="5" width="4.9843137254902"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="5" width="5.4156862745098"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="5" width="4.52941176470588"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="5" width="5.4156862745098"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="5" width="4.83137254901961"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="5" width="4.69411764705882"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="5" width="4.9843137254902"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="5" width="4.52941176470588"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="5" width="4.69411764705882"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="5" width="5.70588235294118"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="5" width="5.4156862745098"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="5" width="4.69411764705882"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="5" width="4.52941176470588"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="5" width="5.27450980392157"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="5" width="5.12941176470588"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="5" width="4.9843137254902"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="5" width="4.24313725490196"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="5" width="4.52941176470588"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="5" width="5.12941176470588"/>
-    <col collapsed="false" hidden="false" max="31" min="30" style="5" width="4.9843137254902"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="5" width="5.56078431372549"/>
-    <col collapsed="false" hidden="false" max="257" min="33" style="0" width="8.89803921568628"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.043137254902"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="5.01176470588235"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="4.72156862745098"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="5.44313725490196"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="5.15686274509804"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="5" width="4.41176470588235"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="4.27058823529412"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="5" width="4.72156862745098"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="5" width="5.01176470588235"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="5" width="5.44313725490196"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="5" width="4.54901960784314"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="5" width="5.44313725490196"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="5" width="4.85490196078431"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="5" width="4.72156862745098"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="5" width="5.01176470588235"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="5" width="4.54901960784314"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="5" width="4.72156862745098"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="5" width="5.73333333333333"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="5" width="5.44313725490196"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="5" width="4.72156862745098"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="5" width="4.54901960784314"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="5" width="5.29803921568627"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="5" width="5.15686274509804"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="5" width="5.01176470588235"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="5" width="4.27058823529412"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="5" width="4.54901960784314"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="5" width="5.15686274509804"/>
+    <col collapsed="false" hidden="false" max="31" min="30" style="5" width="5.01176470588235"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="5" width="5.58823529411765"/>
+    <col collapsed="false" hidden="false" max="257" min="33" style="0" width="8.94509803921569"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
@@ -8389,6 +8404,9 @@
       <c r="D73" s="5" t="n">
         <v>29</v>
       </c>
+      <c r="E73" s="5" t="n">
+        <v>40</v>
+      </c>
       <c r="S73" s="27"/>
       <c r="T73" s="27"/>
     </row>
@@ -8398,10 +8416,10 @@
         <v>1</v>
       </c>
       <c r="C74" s="10"/>
-      <c r="D74" s="10" t="s">
+      <c r="D74" s="10"/>
+      <c r="E74" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="E74" s="10"/>
       <c r="F74" s="10"/>
       <c r="G74" s="7"/>
       <c r="H74" s="10"/>
@@ -8455,41 +8473,41 @@
   <dimension ref="A1:AF71"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A49" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <selection activeCell="D71" activeCellId="0" pane="topLeft" sqref="D71"/>
+      <selection activeCell="F73" activeCellId="0" pane="topLeft" sqref="F73"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9647058823529"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="4.9843137254902"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="4.52941176470588"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="4.08627450980392"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="4.69411764705882"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="5" width="5.27450980392157"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="4.24313725490196"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="5" width="4.69411764705882"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="5" width="4.83137254901961"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="5" width="4.9843137254902"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="5" width="4.52941176470588"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="5" width="5.12941176470588"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="5" width="5.4156862745098"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="5" width="4.9843137254902"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="5" width="4.69411764705882"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="5" width="4.9843137254902"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="5" width="4.52941176470588"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="5" width="4.69411764705882"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="5" width="4.83137254901961"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="5" width="4.52941176470588"/>
-    <col collapsed="false" hidden="false" max="23" min="22" style="5" width="5.12941176470588"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="5" width="5.27450980392157"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="5" width="4.52941176470588"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="5" width="4.69411764705882"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="5" width="5.12941176470588"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="5" width="4.69411764705882"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="5" width="3.95294117647059"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="5" width="3.8"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="5" width="4.83137254901961"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="5" width="5.4156862745098"/>
-    <col collapsed="false" hidden="false" max="257" min="33" style="0" width="8.89803921568628"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.043137254902"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="5.01176470588235"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="4.54901960784314"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="4.10588235294118"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="4.72156862745098"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="5" width="5.29803921568627"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="4.27058823529412"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="5" width="4.72156862745098"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="5" width="4.85490196078431"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="5" width="5.01176470588235"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="5" width="4.54901960784314"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="5" width="5.15686274509804"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="5" width="5.44313725490196"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="5" width="5.01176470588235"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="5" width="4.72156862745098"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="5" width="5.01176470588235"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="5" width="4.54901960784314"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="5" width="4.72156862745098"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="5" width="4.85490196078431"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="5" width="4.54901960784314"/>
+    <col collapsed="false" hidden="false" max="23" min="22" style="5" width="5.15686274509804"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="5" width="5.29803921568627"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="5" width="4.54901960784314"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="5" width="4.72156862745098"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="5" width="5.15686274509804"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="5" width="4.72156862745098"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="5" width="3.96862745098039"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="5" width="3.8156862745098"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="5" width="4.85490196078431"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="5" width="5.44313725490196"/>
+    <col collapsed="false" hidden="false" max="257" min="33" style="0" width="8.94509803921569"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
@@ -10223,7 +10241,7 @@
         <v>20</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="68">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.25" outlineLevel="0" r="68">
       <c r="A68" s="25"/>
       <c r="B68" s="13" t="n">
         <v>7</v>
@@ -10277,10 +10295,10 @@
       <c r="AA68" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="AB68" s="7"/>
-      <c r="AC68" s="7"/>
-      <c r="AD68" s="7"/>
-      <c r="AE68" s="7"/>
+      <c r="AB68" s="11"/>
+      <c r="AC68" s="11"/>
+      <c r="AD68" s="11"/>
+      <c r="AE68" s="11"/>
       <c r="AF68" s="19"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="17.6" outlineLevel="0" r="70">
@@ -10296,17 +10314,24 @@
       <c r="D70" s="5" t="n">
         <v>34</v>
       </c>
+      <c r="E70" s="5" t="n">
+        <v>50</v>
+      </c>
       <c r="S70" s="27"/>
       <c r="T70" s="27"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.25" outlineLevel="0" r="71">
       <c r="A71" s="25"/>
-      <c r="B71" s="7"/>
-      <c r="C71" s="10"/>
-      <c r="D71" s="10" t="s">
+      <c r="B71" s="11"/>
+      <c r="C71" s="13" t="n">
+        <v>6</v>
+      </c>
+      <c r="D71" s="13" t="n">
+        <v>7</v>
+      </c>
+      <c r="E71" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="E71" s="10"/>
       <c r="F71" s="10"/>
       <c r="G71" s="7"/>
       <c r="H71" s="10"/>
@@ -10359,39 +10384,39 @@
   <dimension ref="A1:AF28"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A7" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <selection activeCell="D28" activeCellId="0" pane="topLeft" sqref="D28"/>
+      <selection activeCell="E28" activeCellId="0" pane="topLeft" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9647058823529"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="5.27450980392157"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="4.9843137254902"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="5.12941176470588"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="4.69411764705882"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="5" width="5.27450980392157"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="4.24313725490196"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="5" width="4.69411764705882"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="5" width="5.12941176470588"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="5" width="4.9843137254902"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="5" width="4.52941176470588"/>
-    <col collapsed="false" hidden="false" max="14" min="13" style="5" width="5.4156862745098"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="5" width="4.83137254901961"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="5" width="4.9843137254902"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="5" width="4.24313725490196"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="5" width="5.27450980392157"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="5" width="4.69411764705882"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="5" width="5.27450980392157"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="5" width="5.4156862745098"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="5" width="4.83137254901961"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="5" width="5.4156862745098"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="5" width="4.52941176470588"/>
-    <col collapsed="false" hidden="false" max="26" min="25" style="5" width="4.38823529411765"/>
-    <col collapsed="false" hidden="false" max="28" min="27" style="5" width="4.24313725490196"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="5" width="4.83137254901961"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="5" width="4.9843137254902"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="5" width="4.69411764705882"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="5" width="5.12941176470588"/>
-    <col collapsed="false" hidden="false" max="257" min="33" style="0" width="8.89803921568628"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.043137254902"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="5.29803921568627"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="5.01176470588235"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="5.15686274509804"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="4.72156862745098"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="5" width="5.29803921568627"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="4.27058823529412"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="5" width="4.72156862745098"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="5" width="5.15686274509804"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="5" width="5.01176470588235"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="5" width="4.54901960784314"/>
+    <col collapsed="false" hidden="false" max="14" min="13" style="5" width="5.44313725490196"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="5" width="4.85490196078431"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="5" width="5.01176470588235"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="5" width="4.27058823529412"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="5" width="5.29803921568627"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="5" width="4.72156862745098"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="5" width="5.29803921568627"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="5" width="5.44313725490196"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="5" width="4.85490196078431"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="5" width="5.44313725490196"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="5" width="4.54901960784314"/>
+    <col collapsed="false" hidden="false" max="26" min="25" style="5" width="4.41176470588235"/>
+    <col collapsed="false" hidden="false" max="28" min="27" style="5" width="4.27058823529412"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="5" width="4.85490196078431"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="5" width="5.01176470588235"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="5" width="4.72156862745098"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="5" width="5.15686274509804"/>
+    <col collapsed="false" hidden="false" max="257" min="33" style="0" width="8.94509803921569"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
@@ -11243,6 +11268,9 @@
       <c r="D27" s="5" t="n">
         <v>36</v>
       </c>
+      <c r="E27" s="5" t="n">
+        <v>57</v>
+      </c>
       <c r="S27" s="27"/>
       <c r="T27" s="27"/>
     </row>
@@ -11254,10 +11282,10 @@
       <c r="C28" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="D28" s="10" t="s">
+      <c r="D28" s="10"/>
+      <c r="E28" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="E28" s="10"/>
       <c r="F28" s="10"/>
       <c r="G28" s="7"/>
       <c r="H28" s="10"/>
@@ -11305,42 +11333,42 @@
   <dimension ref="A1:AF39"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A19" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <selection activeCell="D39" activeCellId="0" pane="topLeft" sqref="D39"/>
+      <selection activeCell="E39" activeCellId="0" pane="topLeft" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9647058823529"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="4.24313725490196"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="4.69411764705882"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="4.9843137254902"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="4.69411764705882"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="5" width="5.27450980392157"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="4.24313725490196"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="5" width="5.27450980392157"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="5" width="5.70588235294118"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="5" width="5.4156862745098"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="5" width="4.9843137254902"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="5" width="4.52941176470588"/>
-    <col collapsed="false" hidden="false" max="14" min="13" style="5" width="5.4156862745098"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="5" width="4.38823529411765"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="5" width="4.83137254901961"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="5" width="5.4156862745098"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="5" width="5.84313725490196"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="5" width="4.69411764705882"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="5" width="5.70588235294118"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="5" width="5.4156862745098"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="5" width="5.56078431372549"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="5" width="5.99607843137255"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="5" width="5.4156862745098"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="5" width="4.9843137254902"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="5" width="4.69411764705882"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="5" width="4.24313725490196"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="5" width="4.83137254901961"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="5" width="3.95294117647059"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="5" width="4.69411764705882"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="5" width="5.4156862745098"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="5.56078431372549"/>
-    <col collapsed="false" hidden="false" max="257" min="33" style="0" width="8.89803921568628"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.043137254902"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="4.27058823529412"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="4.72156862745098"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="5.01176470588235"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="4.72156862745098"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="5" width="5.29803921568627"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="4.27058823529412"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="5" width="5.29803921568627"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="5" width="5.73333333333333"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="5" width="5.44313725490196"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="5" width="5.01176470588235"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="5" width="4.54901960784314"/>
+    <col collapsed="false" hidden="false" max="14" min="13" style="5" width="5.44313725490196"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="5" width="4.41176470588235"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="5" width="4.85490196078431"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="5" width="5.44313725490196"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="5" width="5.87058823529412"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="5" width="4.72156862745098"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="5" width="5.73333333333333"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="5" width="5.44313725490196"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="5" width="5.58823529411765"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="5" width="6.02352941176471"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="5" width="5.44313725490196"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="5" width="5.01176470588235"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="5" width="4.72156862745098"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="5" width="4.27058823529412"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="5" width="4.85490196078431"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="5" width="3.96862745098039"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="5" width="4.72156862745098"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="5" width="5.44313725490196"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="5.58823529411765"/>
+    <col collapsed="false" hidden="false" max="257" min="33" style="0" width="8.94509803921569"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
@@ -12699,6 +12727,9 @@
       <c r="D38" s="5" t="n">
         <v>38</v>
       </c>
+      <c r="E38" s="5" t="n">
+        <v>59</v>
+      </c>
       <c r="S38" s="27"/>
       <c r="T38" s="27"/>
       <c r="AF38" s="5"/>
@@ -12711,10 +12742,10 @@
       <c r="C39" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="D39" s="10" t="s">
+      <c r="D39" s="10"/>
+      <c r="E39" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="E39" s="10"/>
       <c r="F39" s="10"/>
       <c r="G39" s="7"/>
       <c r="H39" s="10"/>
@@ -12766,36 +12797,36 @@
   <dimension ref="A1:AF48"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A22" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <selection activeCell="D48" activeCellId="0" pane="topLeft" sqref="D48"/>
+      <selection activeCell="E48" activeCellId="0" pane="topLeft" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9647058823529"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="4.83137254901961"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="3.95294117647059"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="4.08627450980392"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="4.69411764705882"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="5" width="4.52941176470588"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="5" width="4.24313725490196"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="5" width="4.69411764705882"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="5" width="4.9843137254902"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="5" width="4.52941176470588"/>
-    <col collapsed="false" hidden="false" max="14" min="13" style="5" width="5.4156862745098"/>
-    <col collapsed="false" hidden="false" max="17" min="15" style="5" width="4.83137254901961"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="5" width="4.52941176470588"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="5" width="4.69411764705882"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="5" width="5.70588235294118"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="5" width="5.27450980392157"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="5" width="4.83137254901961"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="5" width="4.9843137254902"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="5" width="4.52941176470588"/>
-    <col collapsed="false" hidden="false" max="26" min="25" style="5" width="4.69411764705882"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="5" width="4.24313725490196"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="5" width="4.38823529411765"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="5" width="4.83137254901961"/>
-    <col collapsed="false" hidden="false" max="31" min="30" style="5" width="4.52941176470588"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="5" width="5.12941176470588"/>
-    <col collapsed="false" hidden="false" max="257" min="33" style="0" width="8.89803921568628"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.043137254902"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="4.85490196078431"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="3.96862745098039"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="4.10588235294118"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="4.72156862745098"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="5" width="4.54901960784314"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="5" width="4.27058823529412"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="5" width="4.72156862745098"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="5" width="5.01176470588235"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="5" width="4.54901960784314"/>
+    <col collapsed="false" hidden="false" max="14" min="13" style="5" width="5.44313725490196"/>
+    <col collapsed="false" hidden="false" max="17" min="15" style="5" width="4.85490196078431"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="5" width="4.54901960784314"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="5" width="4.72156862745098"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="5" width="5.73333333333333"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="5" width="5.29803921568627"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="5" width="4.85490196078431"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="5" width="5.01176470588235"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="5" width="4.54901960784314"/>
+    <col collapsed="false" hidden="false" max="26" min="25" style="5" width="4.72156862745098"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="5" width="4.27058823529412"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="5" width="4.41176470588235"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="5" width="4.85490196078431"/>
+    <col collapsed="false" hidden="false" max="31" min="30" style="5" width="4.54901960784314"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="5" width="5.15686274509804"/>
+    <col collapsed="false" hidden="false" max="257" min="33" style="0" width="8.94509803921569"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
@@ -14035,6 +14066,9 @@
       <c r="D47" s="5" t="n">
         <v>38</v>
       </c>
+      <c r="E47" s="5" t="n">
+        <v>71</v>
+      </c>
       <c r="S47" s="27"/>
       <c r="T47" s="27"/>
     </row>
@@ -14042,10 +14076,10 @@
       <c r="A48" s="25"/>
       <c r="B48" s="7"/>
       <c r="C48" s="10"/>
-      <c r="D48" s="10" t="s">
+      <c r="D48" s="10"/>
+      <c r="E48" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="E48" s="10"/>
       <c r="F48" s="10"/>
       <c r="G48" s="7"/>
       <c r="H48" s="10"/>
@@ -14096,37 +14130,37 @@
   <dimension ref="A1:AF69"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A40" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <selection activeCell="D69" activeCellId="0" pane="topLeft" sqref="D69"/>
+      <selection activeCell="E69" activeCellId="0" pane="topLeft" sqref="E69"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9647058823529"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="4.38823529411765"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="5.27450980392157"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="4.08627450980392"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="5" width="4.69411764705882"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="4.24313725490196"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="5" width="4.83137254901961"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="5" width="4.69411764705882"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="5" width="4.9843137254902"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="5" width="4.52941176470588"/>
-    <col collapsed="false" hidden="false" max="14" min="13" style="5" width="5.4156862745098"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="5" width="4.83137254901961"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="5" width="4.69411764705882"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="5" width="5.12941176470588"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="5" width="4.52941176470588"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="5" width="4.69411764705882"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="5" width="5.70588235294118"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="5" width="5.4156862745098"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="5" width="4.83137254901961"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="5" width="4.9843137254902"/>
-    <col collapsed="false" hidden="false" max="25" min="24" style="5" width="4.69411764705882"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="5" width="5.27450980392157"/>
-    <col collapsed="false" hidden="false" max="28" min="27" style="5" width="4.9843137254902"/>
-    <col collapsed="false" hidden="false" max="30" min="29" style="5" width="4.52941176470588"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="5" width="4.24313725490196"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="5" width="4.83137254901961"/>
-    <col collapsed="false" hidden="false" max="257" min="33" style="0" width="8.89803921568628"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.043137254902"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="4.41176470588235"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="5.29803921568627"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="4.10588235294118"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="5" width="4.72156862745098"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="4.27058823529412"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="5" width="4.85490196078431"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="5" width="4.72156862745098"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="5" width="5.01176470588235"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="5" width="4.54901960784314"/>
+    <col collapsed="false" hidden="false" max="14" min="13" style="5" width="5.44313725490196"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="5" width="4.85490196078431"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="5" width="4.72156862745098"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="5" width="5.15686274509804"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="5" width="4.54901960784314"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="5" width="4.72156862745098"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="5" width="5.73333333333333"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="5" width="5.44313725490196"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="5" width="4.85490196078431"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="5" width="5.01176470588235"/>
+    <col collapsed="false" hidden="false" max="25" min="24" style="5" width="4.72156862745098"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="5" width="5.29803921568627"/>
+    <col collapsed="false" hidden="false" max="28" min="27" style="5" width="5.01176470588235"/>
+    <col collapsed="false" hidden="false" max="30" min="29" style="5" width="4.54901960784314"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="5" width="4.27058823529412"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="5" width="4.85490196078431"/>
+    <col collapsed="false" hidden="false" max="257" min="33" style="0" width="8.94509803921569"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
@@ -15980,6 +16014,9 @@
       <c r="D68" s="5" t="n">
         <v>41</v>
       </c>
+      <c r="E68" s="5" t="n">
+        <v>76</v>
+      </c>
       <c r="S68" s="27"/>
       <c r="T68" s="27"/>
     </row>
@@ -15991,10 +16028,12 @@
       <c r="C69" s="10" t="n">
         <v>3</v>
       </c>
-      <c r="D69" s="10" t="s">
+      <c r="D69" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E69" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="E69" s="10"/>
       <c r="F69" s="10"/>
       <c r="G69" s="7"/>
       <c r="H69" s="10"/>

</xml_diff>

<commit_message>
update 05 - 12
</commit_message>
<xml_diff>
--- a/MakeMoney/Thong_Ke/xls/Cau_T2.xlsx
+++ b/MakeMoney/Thong_Ke/xls/Cau_T2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="10" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="499" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="10" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="463" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="CK" sheetId="1" state="visible" r:id="rId2"/>
@@ -530,9 +530,9 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.94509803921569"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.043137254902"/>
-    <col collapsed="false" hidden="false" max="257" min="3" style="0" width="8.94509803921569"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.98823529411765"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.3137254901961"/>
+    <col collapsed="false" hidden="false" max="257" min="3" style="0" width="8.98823529411765"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
@@ -687,41 +687,41 @@
   <dimension ref="A1:AF29"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A10" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <selection activeCell="E29" activeCellId="0" pane="topLeft" sqref="E29"/>
+      <selection activeCell="J32" activeCellId="0" pane="topLeft" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.043137254902"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="4.54901960784314"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="3.96862745098039"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="4.10588235294118"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="4.72156862745098"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="5" width="4.54901960784314"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="4.27058823529412"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="5" width="4.85490196078431"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="5" width="4.72156862745098"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="5" width="4.41176470588235"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="5" width="5.01176470588235"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="5" width="4.54901960784314"/>
-    <col collapsed="false" hidden="false" max="14" min="13" style="5" width="5.44313725490196"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="5" width="4.85490196078431"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="5" width="4.54901960784314"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="5" width="4.85490196078431"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="5" width="4.54901960784314"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="5" width="4.72156862745098"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="5" width="5.73333333333333"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="5" width="5.44313725490196"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="5" width="5.01176470588235"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="5" width="5.44313725490196"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="5" width="5.29803921568627"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="5" width="4.54901960784314"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="5" width="5.15686274509804"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="5" width="4.27058823529412"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="5" width="4.54901960784314"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="5" width="3.96862745098039"/>
-    <col collapsed="false" hidden="false" max="31" min="30" style="5" width="4.72156862745098"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="5" width="5.44313725490196"/>
-    <col collapsed="false" hidden="false" max="257" min="33" style="0" width="8.94509803921569"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.1176470588235"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="4.57647058823529"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="3.98823529411765"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="4.12549019607843"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="4.74117647058824"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="5" width="4.57647058823529"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="4.29411764705882"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="5" width="4.88235294117647"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="5" width="4.74117647058824"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="5" width="4.43137254901961"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="5" width="5.03921568627451"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="5" width="4.57647058823529"/>
+    <col collapsed="false" hidden="false" max="14" min="13" style="5" width="5.47058823529412"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="5" width="4.88235294117647"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="5" width="4.57647058823529"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="5" width="4.88235294117647"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="5" width="4.57647058823529"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="5" width="4.74117647058824"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="5" width="5.76078431372549"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="5" width="5.47058823529412"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="5" width="5.03921568627451"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="5" width="5.47058823529412"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="5" width="5.31764705882353"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="5" width="4.57647058823529"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="5" width="5.1843137254902"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="5" width="4.29411764705882"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="5" width="4.57647058823529"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="5" width="3.98823529411765"/>
+    <col collapsed="false" hidden="false" max="31" min="30" style="5" width="4.74117647058824"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="5" width="5.47058823529412"/>
+    <col collapsed="false" hidden="false" max="257" min="33" style="0" width="8.98823529411765"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
@@ -1586,6 +1586,9 @@
       <c r="E28" s="5" t="n">
         <v>81</v>
       </c>
+      <c r="F28" s="5" t="n">
+        <v>87</v>
+      </c>
       <c r="S28" s="27"/>
       <c r="T28" s="27"/>
     </row>
@@ -1596,10 +1599,12 @@
       <c r="D29" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="E29" s="10" t="s">
+      <c r="E29" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="F29" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="F29" s="10"/>
       <c r="G29" s="7"/>
       <c r="H29" s="10"/>
       <c r="I29" s="10"/>
@@ -1646,40 +1651,40 @@
   <dimension ref="A1:AF65"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A43" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <selection activeCell="E65" activeCellId="0" pane="topLeft" sqref="E65"/>
+      <selection activeCell="G67" activeCellId="0" pane="topLeft" sqref="G67"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.043137254902"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="4.41176470588235"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="4.54901960784314"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="4.10588235294118"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="4.72156862745098"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="5" width="4.41176470588235"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="4.27058823529412"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="5" width="5.01176470588235"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="5" width="4.72156862745098"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="5" width="4.54901960784314"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="5" width="5.01176470588235"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="5" width="4.54901960784314"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="5" width="4.72156862745098"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="5" width="5.44313725490196"/>
-    <col collapsed="false" hidden="false" max="16" min="15" style="5" width="4.72156862745098"/>
-    <col collapsed="false" hidden="false" max="18" min="17" style="5" width="5.01176470588235"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="5" width="4.72156862745098"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="5" width="5.73333333333333"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="5" width="5.44313725490196"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="5" width="5.58823529411765"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="5" width="5.44313725490196"/>
-    <col collapsed="false" hidden="false" max="25" min="24" style="5" width="5.01176470588235"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="5" width="4.41176470588235"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="5" width="4.27058823529412"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="5" width="4.72156862745098"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="5" width="3.96862745098039"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="5" width="4.10588235294118"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="5" width="4.54901960784314"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="5" width="3.8156862745098"/>
-    <col collapsed="false" hidden="false" max="257" min="33" style="0" width="8.94509803921569"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.1176470588235"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="4.43137254901961"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="4.57647058823529"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="4.12549019607843"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="4.74117647058824"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="5" width="4.43137254901961"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="4.29411764705882"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="5" width="5.03921568627451"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="5" width="4.74117647058824"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="5" width="4.57647058823529"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="5" width="5.03921568627451"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="5" width="4.57647058823529"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="5" width="4.74117647058824"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="5" width="5.47058823529412"/>
+    <col collapsed="false" hidden="false" max="16" min="15" style="5" width="4.74117647058824"/>
+    <col collapsed="false" hidden="false" max="18" min="17" style="5" width="5.03921568627451"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="5" width="4.74117647058824"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="5" width="5.76078431372549"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="5" width="5.47058823529412"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="5" width="5.6156862745098"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="5" width="5.47058823529412"/>
+    <col collapsed="false" hidden="false" max="25" min="24" style="5" width="5.03921568627451"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="5" width="4.43137254901961"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="5" width="4.29411764705882"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="5" width="4.74117647058824"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="5" width="3.98823529411765"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="5" width="4.12549019607843"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="5" width="4.57647058823529"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="5" width="3.83529411764706"/>
+    <col collapsed="false" hidden="false" max="257" min="33" style="0" width="8.98823529411765"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
@@ -3525,7 +3530,9 @@
       <c r="E65" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="F65" s="10"/>
+      <c r="F65" s="10" t="n">
+        <v>0</v>
+      </c>
       <c r="G65" s="7"/>
       <c r="H65" s="10"/>
       <c r="I65" s="10"/>
@@ -3576,39 +3583,39 @@
   <dimension ref="A1:AF69"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A58" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <selection activeCell="E69" activeCellId="0" pane="topLeft" sqref="E69"/>
+      <selection activeCell="F69" activeCellId="0" pane="topLeft" sqref="F69"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.043137254902"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="5.29803921568627"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="6.17647058823529"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="5.44313725490196"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="5" width="5.58823529411765"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="5.29803921568627"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="5" width="5.58823529411765"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="5" width="5.73333333333333"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="5" width="5.58823529411765"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="5" width="5.01176470588235"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="5" width="5.58823529411765"/>
-    <col collapsed="false" hidden="false" max="16" min="13" style="5" width="5.44313725490196"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="5" width="5.58823529411765"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="5" width="4.72156862745098"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="5" width="5.01176470588235"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="5" width="5.87058823529412"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="5" width="5.73333333333333"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="5" width="5.37254901960784"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="5" width="5.52549019607843"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="5" width="5.21960784313726"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="5" width="5.67843137254902"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="5" width="5.21960784313726"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="5" width="5.87058823529412"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="5" width="4.72156862745098"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="5" width="4.41176470588235"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="5" width="4.27058823529412"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="5" width="4.72156862745098"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="5" width="4.85490196078431"/>
-    <col collapsed="false" hidden="false" max="257" min="33" style="0" width="8.94509803921569"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.1176470588235"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="5.31764705882353"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="6.21176470588235"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="5.47058823529412"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="5" width="5.6156862745098"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="5.31764705882353"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="5" width="5.6156862745098"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="5" width="5.76078431372549"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="5" width="5.6156862745098"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="5" width="5.03921568627451"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="5" width="5.6156862745098"/>
+    <col collapsed="false" hidden="false" max="16" min="13" style="5" width="5.47058823529412"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="5" width="5.6156862745098"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="5" width="4.74117647058824"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="5" width="5.03921568627451"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="5" width="5.90588235294118"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="5" width="5.76078431372549"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="5" width="5.4"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="5" width="5.55294117647059"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="5" width="5.24705882352941"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="5" width="5.70588235294118"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="5" width="5.24705882352941"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="5" width="5.90588235294118"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="5" width="4.74117647058824"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="5" width="4.43137254901961"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="5" width="4.29411764705882"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="5" width="4.74117647058824"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="5" width="4.88235294117647"/>
+    <col collapsed="false" hidden="false" max="257" min="33" style="0" width="8.98823529411765"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
@@ -5371,7 +5378,7 @@
         <v>42</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.25" outlineLevel="0" r="66">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="66">
       <c r="A66" s="25"/>
       <c r="B66" s="7" t="n">
         <v>2</v>
@@ -5447,6 +5454,9 @@
       <c r="E68" s="5" t="n">
         <v>19</v>
       </c>
+      <c r="F68" s="5" t="n">
+        <v>90</v>
+      </c>
       <c r="S68" s="27"/>
       <c r="T68" s="27"/>
     </row>
@@ -5459,10 +5469,12 @@
       <c r="D69" s="13" t="n">
         <v>7</v>
       </c>
-      <c r="E69" s="10" t="s">
+      <c r="E69" s="13" t="n">
+        <v>8</v>
+      </c>
+      <c r="F69" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="F69" s="10"/>
       <c r="G69" s="7"/>
       <c r="H69" s="10"/>
       <c r="I69" s="10"/>
@@ -5513,39 +5525,39 @@
   <dimension ref="A1:AF30"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <selection activeCell="E30" activeCellId="0" pane="topLeft" sqref="E30"/>
+      <selection activeCell="F30" activeCellId="0" pane="topLeft" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.9921568627451"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="4.85490196078431"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="5" width="5.58823529411765"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="6.34117647058824"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="5" width="5.29803921568627"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="5" width="5.01176470588235"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="5" width="4.72156862745098"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="5" width="5.29803921568627"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="5" width="5.01176470588235"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="5" width="4.54901960784314"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="5" width="4.85490196078431"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="5" width="4.72156862745098"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="5" width="5.73333333333333"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="5" width="5.29803921568627"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="5" width="5.58823529411765"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="5" width="5.73333333333333"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="5" width="6.17647058823529"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="5" width="5.73333333333333"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="5" width="5.44313725490196"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="5" width="5.58823529411765"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="5" width="5.15686274509804"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="5" width="5.01176470588235"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="5" width="5.15686274509804"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="5" width="5.29803921568627"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="5" width="4.85490196078431"/>
-    <col collapsed="false" hidden="false" max="30" min="28" style="5" width="5.15686274509804"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="5" width="4.41176470588235"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="5" width="5.73333333333333"/>
-    <col collapsed="false" hidden="false" max="257" min="33" style="0" width="8.94509803921569"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.0627450980392"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="4.88235294117647"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="5" width="5.6156862745098"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="6.37647058823529"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="5" width="5.31764705882353"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="5" width="5.03921568627451"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="5" width="4.74117647058824"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="5" width="5.31764705882353"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="5" width="5.03921568627451"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="5" width="4.57647058823529"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="5" width="4.88235294117647"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="5" width="4.74117647058824"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="5" width="5.76078431372549"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="5" width="5.31764705882353"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="5" width="5.6156862745098"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="5" width="5.76078431372549"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="5" width="6.21176470588235"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="5" width="5.76078431372549"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="5" width="5.47058823529412"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="5" width="5.6156862745098"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="5" width="5.1843137254902"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="5" width="5.03921568627451"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="5" width="5.1843137254902"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="5" width="5.31764705882353"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="5" width="4.88235294117647"/>
+    <col collapsed="false" hidden="false" max="30" min="28" style="5" width="5.1843137254902"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="5" width="4.43137254901961"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="5" width="5.76078431372549"/>
+    <col collapsed="false" hidden="false" max="257" min="33" style="0" width="8.98823529411765"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
@@ -6430,6 +6442,9 @@
       <c r="E29" s="5" t="n">
         <v>24</v>
       </c>
+      <c r="F29" s="5" t="n">
+        <v>38</v>
+      </c>
       <c r="S29" s="27"/>
       <c r="T29" s="27"/>
     </row>
@@ -6442,10 +6457,12 @@
         <v>1</v>
       </c>
       <c r="D30" s="10"/>
-      <c r="E30" s="10" t="s">
+      <c r="E30" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="F30" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="F30" s="10"/>
       <c r="G30" s="7"/>
       <c r="H30" s="10"/>
       <c r="I30" s="10"/>
@@ -6492,40 +6509,40 @@
   <dimension ref="A1:AF74"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A58" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <selection activeCell="E74" activeCellId="0" pane="topLeft" sqref="E74"/>
+      <selection activeCell="F74" activeCellId="0" pane="topLeft" sqref="F74"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.043137254902"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="5.01176470588235"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="4.72156862745098"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="5.44313725490196"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="5.15686274509804"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="5" width="4.41176470588235"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="4.27058823529412"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="5" width="4.72156862745098"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="5" width="5.01176470588235"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="5" width="5.44313725490196"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="5" width="4.54901960784314"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="5" width="5.44313725490196"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="5" width="4.85490196078431"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="5" width="4.72156862745098"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="5" width="5.01176470588235"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="5" width="4.54901960784314"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="5" width="4.72156862745098"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="5" width="5.73333333333333"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="5" width="5.44313725490196"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="5" width="4.72156862745098"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="5" width="4.54901960784314"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="5" width="5.29803921568627"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="5" width="5.15686274509804"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="5" width="5.01176470588235"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="5" width="4.27058823529412"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="5" width="4.54901960784314"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="5" width="5.15686274509804"/>
-    <col collapsed="false" hidden="false" max="31" min="30" style="5" width="5.01176470588235"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="5" width="5.58823529411765"/>
-    <col collapsed="false" hidden="false" max="257" min="33" style="0" width="8.94509803921569"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.1176470588235"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="5.03921568627451"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="4.74117647058824"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="5.47058823529412"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="5.1843137254902"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="5" width="4.43137254901961"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="4.29411764705882"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="5" width="4.74117647058824"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="5" width="5.03921568627451"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="5" width="5.47058823529412"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="5" width="4.57647058823529"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="5" width="5.47058823529412"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="5" width="4.88235294117647"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="5" width="4.74117647058824"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="5" width="5.03921568627451"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="5" width="4.57647058823529"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="5" width="4.74117647058824"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="5" width="5.76078431372549"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="5" width="5.47058823529412"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="5" width="4.74117647058824"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="5" width="4.57647058823529"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="5" width="5.31764705882353"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="5" width="5.1843137254902"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="5" width="5.03921568627451"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="5" width="4.29411764705882"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="5" width="4.57647058823529"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="5" width="5.1843137254902"/>
+    <col collapsed="false" hidden="false" max="31" min="30" style="5" width="5.03921568627451"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="5" width="5.6156862745098"/>
+    <col collapsed="false" hidden="false" max="257" min="33" style="0" width="8.98823529411765"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
@@ -8407,6 +8424,9 @@
       <c r="E73" s="5" t="n">
         <v>40</v>
       </c>
+      <c r="F73" s="5" t="n">
+        <v>41</v>
+      </c>
       <c r="S73" s="27"/>
       <c r="T73" s="27"/>
     </row>
@@ -8417,10 +8437,10 @@
       </c>
       <c r="C74" s="10"/>
       <c r="D74" s="10"/>
-      <c r="E74" s="10" t="s">
+      <c r="E74" s="10"/>
+      <c r="F74" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="F74" s="10"/>
       <c r="G74" s="7"/>
       <c r="H74" s="10"/>
       <c r="I74" s="10"/>
@@ -8473,41 +8493,41 @@
   <dimension ref="A1:AF71"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A49" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <selection activeCell="F73" activeCellId="0" pane="topLeft" sqref="F73"/>
+      <selection activeCell="F71" activeCellId="0" pane="topLeft" sqref="F71"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.043137254902"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="5.01176470588235"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="4.54901960784314"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="4.10588235294118"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="4.72156862745098"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="5" width="5.29803921568627"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="4.27058823529412"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="5" width="4.72156862745098"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="5" width="4.85490196078431"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="5" width="5.01176470588235"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="5" width="4.54901960784314"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="5" width="5.15686274509804"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="5" width="5.44313725490196"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="5" width="5.01176470588235"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="5" width="4.72156862745098"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="5" width="5.01176470588235"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="5" width="4.54901960784314"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="5" width="4.72156862745098"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="5" width="4.85490196078431"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="5" width="4.54901960784314"/>
-    <col collapsed="false" hidden="false" max="23" min="22" style="5" width="5.15686274509804"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="5" width="5.29803921568627"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="5" width="4.54901960784314"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="5" width="4.72156862745098"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="5" width="5.15686274509804"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="5" width="4.72156862745098"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="5" width="3.96862745098039"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="5" width="3.8156862745098"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="5" width="4.85490196078431"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="5" width="5.44313725490196"/>
-    <col collapsed="false" hidden="false" max="257" min="33" style="0" width="8.94509803921569"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.1176470588235"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="5.03921568627451"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="4.57647058823529"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="4.12549019607843"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="4.74117647058824"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="5" width="5.31764705882353"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="4.29411764705882"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="5" width="4.74117647058824"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="5" width="4.88235294117647"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="5" width="5.03921568627451"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="5" width="4.57647058823529"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="5" width="5.1843137254902"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="5" width="5.47058823529412"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="5" width="5.03921568627451"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="5" width="4.74117647058824"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="5" width="5.03921568627451"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="5" width="4.57647058823529"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="5" width="4.74117647058824"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="5" width="4.88235294117647"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="5" width="4.57647058823529"/>
+    <col collapsed="false" hidden="false" max="23" min="22" style="5" width="5.1843137254902"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="5" width="5.31764705882353"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="5" width="4.57647058823529"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="5" width="4.74117647058824"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="5" width="5.1843137254902"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="5" width="4.74117647058824"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="5" width="3.98823529411765"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="5" width="3.83529411764706"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="5" width="4.88235294117647"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="5" width="5.47058823529412"/>
+    <col collapsed="false" hidden="false" max="257" min="33" style="0" width="8.98823529411765"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
@@ -10241,7 +10261,7 @@
         <v>20</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.25" outlineLevel="0" r="68">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="68">
       <c r="A68" s="25"/>
       <c r="B68" s="13" t="n">
         <v>7</v>
@@ -10317,6 +10337,9 @@
       <c r="E70" s="5" t="n">
         <v>50</v>
       </c>
+      <c r="F70" s="5" t="n">
+        <v>44</v>
+      </c>
       <c r="S70" s="27"/>
       <c r="T70" s="27"/>
     </row>
@@ -10329,10 +10352,12 @@
       <c r="D71" s="13" t="n">
         <v>7</v>
       </c>
-      <c r="E71" s="10" t="s">
+      <c r="E71" s="13" t="n">
+        <v>8</v>
+      </c>
+      <c r="F71" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="F71" s="10"/>
       <c r="G71" s="7"/>
       <c r="H71" s="10"/>
       <c r="I71" s="10"/>
@@ -10384,39 +10409,39 @@
   <dimension ref="A1:AF28"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A7" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <selection activeCell="E28" activeCellId="0" pane="topLeft" sqref="E28"/>
+      <selection activeCell="F28" activeCellId="0" pane="topLeft" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.043137254902"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="5.29803921568627"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="5.01176470588235"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="5.15686274509804"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="4.72156862745098"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="5" width="5.29803921568627"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="4.27058823529412"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="5" width="4.72156862745098"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="5" width="5.15686274509804"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="5" width="5.01176470588235"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="5" width="4.54901960784314"/>
-    <col collapsed="false" hidden="false" max="14" min="13" style="5" width="5.44313725490196"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="5" width="4.85490196078431"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="5" width="5.01176470588235"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="5" width="4.27058823529412"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="5" width="5.29803921568627"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="5" width="4.72156862745098"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="5" width="5.29803921568627"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="5" width="5.44313725490196"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="5" width="4.85490196078431"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="5" width="5.44313725490196"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="5" width="4.54901960784314"/>
-    <col collapsed="false" hidden="false" max="26" min="25" style="5" width="4.41176470588235"/>
-    <col collapsed="false" hidden="false" max="28" min="27" style="5" width="4.27058823529412"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="5" width="4.85490196078431"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="5" width="5.01176470588235"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="5" width="4.72156862745098"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="5" width="5.15686274509804"/>
-    <col collapsed="false" hidden="false" max="257" min="33" style="0" width="8.94509803921569"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.1176470588235"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="5.31764705882353"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="5.03921568627451"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="5.1843137254902"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="4.74117647058824"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="5" width="5.31764705882353"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="4.29411764705882"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="5" width="4.74117647058824"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="5" width="5.1843137254902"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="5" width="5.03921568627451"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="5" width="4.57647058823529"/>
+    <col collapsed="false" hidden="false" max="14" min="13" style="5" width="5.47058823529412"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="5" width="4.88235294117647"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="5" width="5.03921568627451"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="5" width="4.29411764705882"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="5" width="5.31764705882353"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="5" width="4.74117647058824"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="5" width="5.31764705882353"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="5" width="5.47058823529412"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="5" width="4.88235294117647"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="5" width="5.47058823529412"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="5" width="4.57647058823529"/>
+    <col collapsed="false" hidden="false" max="26" min="25" style="5" width="4.43137254901961"/>
+    <col collapsed="false" hidden="false" max="28" min="27" style="5" width="4.29411764705882"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="5" width="4.88235294117647"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="5" width="5.03921568627451"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="5" width="4.74117647058824"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="5" width="5.1843137254902"/>
+    <col collapsed="false" hidden="false" max="257" min="33" style="0" width="8.98823529411765"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
@@ -11271,6 +11296,9 @@
       <c r="E27" s="5" t="n">
         <v>57</v>
       </c>
+      <c r="F27" s="5" t="n">
+        <v>45</v>
+      </c>
       <c r="S27" s="27"/>
       <c r="T27" s="27"/>
     </row>
@@ -11283,10 +11311,10 @@
         <v>1</v>
       </c>
       <c r="D28" s="10"/>
-      <c r="E28" s="10" t="s">
+      <c r="E28" s="10"/>
+      <c r="F28" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="F28" s="10"/>
       <c r="G28" s="7"/>
       <c r="H28" s="10"/>
       <c r="I28" s="10"/>
@@ -11333,42 +11361,42 @@
   <dimension ref="A1:AF39"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A19" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <selection activeCell="E39" activeCellId="0" pane="topLeft" sqref="E39"/>
+      <selection activeCell="F39" activeCellId="0" pane="topLeft" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.043137254902"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="4.27058823529412"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="4.72156862745098"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="5.01176470588235"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="4.72156862745098"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="5" width="5.29803921568627"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="4.27058823529412"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="5" width="5.29803921568627"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="5" width="5.73333333333333"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="5" width="5.44313725490196"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="5" width="5.01176470588235"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="5" width="4.54901960784314"/>
-    <col collapsed="false" hidden="false" max="14" min="13" style="5" width="5.44313725490196"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="5" width="4.41176470588235"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="5" width="4.85490196078431"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="5" width="5.44313725490196"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="5" width="5.87058823529412"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="5" width="4.72156862745098"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="5" width="5.73333333333333"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="5" width="5.44313725490196"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="5" width="5.58823529411765"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="5" width="6.02352941176471"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="5" width="5.44313725490196"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="5" width="5.01176470588235"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="5" width="4.72156862745098"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="5" width="4.27058823529412"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="5" width="4.85490196078431"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="5" width="3.96862745098039"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="5" width="4.72156862745098"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="5" width="5.44313725490196"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="5.58823529411765"/>
-    <col collapsed="false" hidden="false" max="257" min="33" style="0" width="8.94509803921569"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.1176470588235"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="4.29411764705882"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="4.74117647058824"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="5.03921568627451"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="4.74117647058824"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="5" width="5.31764705882353"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="4.29411764705882"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="5" width="5.31764705882353"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="5" width="5.76078431372549"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="5" width="5.47058823529412"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="5" width="5.03921568627451"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="5" width="4.57647058823529"/>
+    <col collapsed="false" hidden="false" max="14" min="13" style="5" width="5.47058823529412"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="5" width="4.43137254901961"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="5" width="4.88235294117647"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="5" width="5.47058823529412"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="5" width="5.90588235294118"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="5" width="4.74117647058824"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="5" width="5.76078431372549"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="5" width="5.47058823529412"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="5" width="5.6156862745098"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="5" width="6.05882352941176"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="5" width="5.47058823529412"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="5" width="5.03921568627451"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="5" width="4.74117647058824"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="5" width="4.29411764705882"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="5" width="4.88235294117647"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="5" width="3.98823529411765"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="5" width="4.74117647058824"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="5" width="5.47058823529412"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="5.6156862745098"/>
+    <col collapsed="false" hidden="false" max="257" min="33" style="0" width="8.98823529411765"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
@@ -12730,6 +12758,9 @@
       <c r="E38" s="5" t="n">
         <v>59</v>
       </c>
+      <c r="F38" s="5" t="n">
+        <v>45</v>
+      </c>
       <c r="S38" s="27"/>
       <c r="T38" s="27"/>
       <c r="AF38" s="5"/>
@@ -12743,10 +12774,10 @@
         <v>1</v>
       </c>
       <c r="D39" s="10"/>
-      <c r="E39" s="10" t="s">
+      <c r="E39" s="10"/>
+      <c r="F39" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="F39" s="10"/>
       <c r="G39" s="7"/>
       <c r="H39" s="10"/>
       <c r="I39" s="10"/>
@@ -12796,37 +12827,37 @@
   </sheetPr>
   <dimension ref="A1:AF48"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A22" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <selection activeCell="E48" activeCellId="0" pane="topLeft" sqref="E48"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A31" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
+      <selection activeCell="F48" activeCellId="0" pane="topLeft" sqref="F48"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.043137254902"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="4.85490196078431"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="3.96862745098039"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="4.10588235294118"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="4.72156862745098"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="5" width="4.54901960784314"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="5" width="4.27058823529412"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="5" width="4.72156862745098"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="5" width="5.01176470588235"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="5" width="4.54901960784314"/>
-    <col collapsed="false" hidden="false" max="14" min="13" style="5" width="5.44313725490196"/>
-    <col collapsed="false" hidden="false" max="17" min="15" style="5" width="4.85490196078431"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="5" width="4.54901960784314"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="5" width="4.72156862745098"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="5" width="5.73333333333333"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="5" width="5.29803921568627"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="5" width="4.85490196078431"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="5" width="5.01176470588235"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="5" width="4.54901960784314"/>
-    <col collapsed="false" hidden="false" max="26" min="25" style="5" width="4.72156862745098"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="5" width="4.27058823529412"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="5" width="4.41176470588235"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="5" width="4.85490196078431"/>
-    <col collapsed="false" hidden="false" max="31" min="30" style="5" width="4.54901960784314"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="5" width="5.15686274509804"/>
-    <col collapsed="false" hidden="false" max="257" min="33" style="0" width="8.94509803921569"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.1176470588235"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="4.88235294117647"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="3.98823529411765"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="4.12549019607843"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="4.74117647058824"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="5" width="4.57647058823529"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="5" width="4.29411764705882"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="5" width="4.74117647058824"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="5" width="5.03921568627451"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="5" width="4.57647058823529"/>
+    <col collapsed="false" hidden="false" max="14" min="13" style="5" width="5.47058823529412"/>
+    <col collapsed="false" hidden="false" max="17" min="15" style="5" width="4.88235294117647"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="5" width="4.57647058823529"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="5" width="4.74117647058824"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="5" width="5.76078431372549"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="5" width="5.31764705882353"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="5" width="4.88235294117647"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="5" width="5.03921568627451"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="5" width="4.57647058823529"/>
+    <col collapsed="false" hidden="false" max="26" min="25" style="5" width="4.74117647058824"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="5" width="4.29411764705882"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="5" width="4.43137254901961"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="5" width="4.88235294117647"/>
+    <col collapsed="false" hidden="false" max="31" min="30" style="5" width="4.57647058823529"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="5" width="5.1843137254902"/>
+    <col collapsed="false" hidden="false" max="257" min="33" style="0" width="8.98823529411765"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
@@ -14069,6 +14100,9 @@
       <c r="E47" s="5" t="n">
         <v>71</v>
       </c>
+      <c r="F47" s="5" t="n">
+        <v>54</v>
+      </c>
       <c r="S47" s="27"/>
       <c r="T47" s="27"/>
     </row>
@@ -14077,10 +14111,10 @@
       <c r="B48" s="7"/>
       <c r="C48" s="10"/>
       <c r="D48" s="10"/>
-      <c r="E48" s="10" t="s">
+      <c r="E48" s="10"/>
+      <c r="F48" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="F48" s="10"/>
       <c r="G48" s="7"/>
       <c r="H48" s="10"/>
       <c r="I48" s="10"/>
@@ -14130,37 +14164,37 @@
   <dimension ref="A1:AF69"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A40" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <selection activeCell="E69" activeCellId="0" pane="topLeft" sqref="E69"/>
+      <selection activeCell="F69" activeCellId="0" pane="topLeft" sqref="F69"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.043137254902"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="4.41176470588235"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="5.29803921568627"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="4.10588235294118"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="5" width="4.72156862745098"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="4.27058823529412"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="5" width="4.85490196078431"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="5" width="4.72156862745098"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="5" width="5.01176470588235"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="5" width="4.54901960784314"/>
-    <col collapsed="false" hidden="false" max="14" min="13" style="5" width="5.44313725490196"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="5" width="4.85490196078431"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="5" width="4.72156862745098"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="5" width="5.15686274509804"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="5" width="4.54901960784314"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="5" width="4.72156862745098"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="5" width="5.73333333333333"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="5" width="5.44313725490196"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="5" width="4.85490196078431"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="5" width="5.01176470588235"/>
-    <col collapsed="false" hidden="false" max="25" min="24" style="5" width="4.72156862745098"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="5" width="5.29803921568627"/>
-    <col collapsed="false" hidden="false" max="28" min="27" style="5" width="5.01176470588235"/>
-    <col collapsed="false" hidden="false" max="30" min="29" style="5" width="4.54901960784314"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="5" width="4.27058823529412"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="5" width="4.85490196078431"/>
-    <col collapsed="false" hidden="false" max="257" min="33" style="0" width="8.94509803921569"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.1176470588235"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="4.43137254901961"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="5.31764705882353"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="4.12549019607843"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="5" width="4.74117647058824"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="4.29411764705882"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="5" width="4.88235294117647"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="5" width="4.74117647058824"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="5" width="5.03921568627451"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="5" width="4.57647058823529"/>
+    <col collapsed="false" hidden="false" max="14" min="13" style="5" width="5.47058823529412"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="5" width="4.88235294117647"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="5" width="4.74117647058824"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="5" width="5.1843137254902"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="5" width="4.57647058823529"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="5" width="4.74117647058824"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="5" width="5.76078431372549"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="5" width="5.47058823529412"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="5" width="4.88235294117647"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="5" width="5.03921568627451"/>
+    <col collapsed="false" hidden="false" max="25" min="24" style="5" width="4.74117647058824"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="5" width="5.31764705882353"/>
+    <col collapsed="false" hidden="false" max="28" min="27" style="5" width="5.03921568627451"/>
+    <col collapsed="false" hidden="false" max="30" min="29" style="5" width="4.57647058823529"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="5" width="4.29411764705882"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="5" width="4.88235294117647"/>
+    <col collapsed="false" hidden="false" max="257" min="33" style="0" width="8.98823529411765"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
@@ -16017,6 +16051,9 @@
       <c r="E68" s="5" t="n">
         <v>76</v>
       </c>
+      <c r="F68" s="5" t="n">
+        <v>62</v>
+      </c>
       <c r="S68" s="27"/>
       <c r="T68" s="27"/>
     </row>
@@ -16031,10 +16068,10 @@
       <c r="D69" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="E69" s="10" t="s">
+      <c r="E69" s="10"/>
+      <c r="F69" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="F69" s="10"/>
       <c r="G69" s="7"/>
       <c r="H69" s="10"/>
       <c r="I69" s="10"/>

</xml_diff>

<commit_message>
update cau so 4
</commit_message>
<xml_diff>
--- a/MakeMoney/Thong_Ke/xls/Cau_T2.xlsx
+++ b/MakeMoney/Thong_Ke/xls/Cau_T2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="2" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="466" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="2" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="526" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="CK" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="56">
   <si>
     <t>Cau so 10</t>
   </si>
@@ -341,7 +341,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
@@ -426,6 +426,9 @@
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
@@ -535,13 +538,13 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="AE3:AF3 A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.68235294117647"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="56.7098039215686"/>
-    <col collapsed="false" hidden="false" max="257" min="3" style="0" width="8.68235294117647"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.72941176470588"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="56.9882352941176"/>
+    <col collapsed="false" hidden="false" max="257" min="3" style="0" width="8.72941176470588"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
@@ -696,41 +699,41 @@
   <dimension ref="A1:AF29"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A4" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <selection activeCell="P31" activeCellId="0" pane="topLeft" sqref="P31"/>
+      <selection activeCell="P31" activeCellId="1" pane="topLeft" sqref="AE3:AF3 P31"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.5254901960784"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="4.69411764705882"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="4.08627450980392"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="4.22352941176471"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="4.85490196078431"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="5" width="4.69411764705882"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="4.38823529411765"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="5" width="5.01176470588235"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="5" width="4.85490196078431"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="5" width="4.54901960784314"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="5" width="5.16470588235294"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="5" width="4.69411764705882"/>
-    <col collapsed="false" hidden="false" max="14" min="13" style="5" width="5.6078431372549"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="5" width="5.01176470588235"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="5" width="4.69411764705882"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="5" width="5.01176470588235"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="5" width="4.69411764705882"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="5" width="4.85490196078431"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="5" width="5.90588235294118"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="5" width="5.6078431372549"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="5" width="5.16470588235294"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="5" width="5.6078431372549"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="5" width="5.45490196078431"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="5" width="4.69411764705882"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="5" width="5.31764705882353"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="5" width="4.38823529411765"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="5" width="4.69411764705882"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="5" width="4.08627450980392"/>
-    <col collapsed="false" hidden="false" max="31" min="30" style="5" width="4.85490196078431"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="5" width="5.6078431372549"/>
-    <col collapsed="false" hidden="false" max="257" min="33" style="0" width="8.68235294117647"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.6039215686275"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="4.72156862745098"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="4.10588235294118"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="4.24313725490196"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="4.88235294117647"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="5" width="4.72156862745098"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="4.41176470588235"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="5" width="5.03921568627451"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="5" width="4.88235294117647"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="5" width="4.57647058823529"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="5" width="5.1921568627451"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="5" width="4.72156862745098"/>
+    <col collapsed="false" hidden="false" max="14" min="13" style="5" width="5.63529411764706"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="5" width="5.03921568627451"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="5" width="4.72156862745098"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="5" width="5.03921568627451"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="5" width="4.72156862745098"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="5" width="4.88235294117647"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="5" width="5.94117647058824"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="5" width="5.63529411764706"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="5" width="5.1921568627451"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="5" width="5.63529411764706"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="5" width="5.48235294117647"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="5" width="4.72156862745098"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="5" width="5.34509803921569"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="5" width="4.41176470588235"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="5" width="4.72156862745098"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="5" width="4.10588235294118"/>
+    <col collapsed="false" hidden="false" max="31" min="30" style="5" width="4.88235294117647"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="5" width="5.63529411764706"/>
+    <col collapsed="false" hidden="false" max="257" min="33" style="0" width="8.72941176470588"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
@@ -1628,7 +1631,7 @@
       <c r="S28" s="27"/>
       <c r="T28" s="27"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.25" outlineLevel="0" r="29">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="29">
       <c r="A29" s="25"/>
       <c r="B29" s="7"/>
       <c r="C29" s="10"/>
@@ -1691,40 +1694,40 @@
   <dimension ref="A1:AF65"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <selection activeCell="P68" activeCellId="0" pane="topLeft" sqref="P68"/>
+      <selection activeCell="P68" activeCellId="1" pane="topLeft" sqref="AE3:AF3 P68"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.5254901960784"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="4.54901960784314"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="4.69411764705882"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="4.22352941176471"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="4.85490196078431"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="5" width="4.54901960784314"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="4.38823529411765"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="5" width="5.16470588235294"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="5" width="4.85490196078431"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="5" width="4.69411764705882"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="5" width="5.16470588235294"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="5" width="4.69411764705882"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="5" width="4.85490196078431"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="5" width="5.6078431372549"/>
-    <col collapsed="false" hidden="false" max="16" min="15" style="5" width="4.85490196078431"/>
-    <col collapsed="false" hidden="false" max="18" min="17" style="5" width="5.16470588235294"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="5" width="4.85490196078431"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="5" width="5.90588235294118"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="5" width="5.6078431372549"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="5" width="5.75294117647059"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="5" width="5.6078431372549"/>
-    <col collapsed="false" hidden="false" max="25" min="24" style="5" width="5.16470588235294"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="5" width="4.54901960784314"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="5" width="4.38823529411765"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="5" width="4.85490196078431"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="5" width="4.08627450980392"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="5" width="4.22352941176471"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="5" width="4.69411764705882"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="5" width="3.92549019607843"/>
-    <col collapsed="false" hidden="false" max="257" min="33" style="0" width="8.68235294117647"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.6039215686275"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="4.57647058823529"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="4.72156862745098"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="4.24313725490196"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="4.88235294117647"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="5" width="4.57647058823529"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="4.41176470588235"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="5" width="5.1921568627451"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="5" width="4.88235294117647"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="5" width="4.72156862745098"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="5" width="5.1921568627451"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="5" width="4.72156862745098"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="5" width="4.88235294117647"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="5" width="5.63529411764706"/>
+    <col collapsed="false" hidden="false" max="16" min="15" style="5" width="4.88235294117647"/>
+    <col collapsed="false" hidden="false" max="18" min="17" style="5" width="5.1921568627451"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="5" width="4.88235294117647"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="5" width="5.94117647058824"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="5" width="5.63529411764706"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="5" width="5.78039215686275"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="5" width="5.63529411764706"/>
+    <col collapsed="false" hidden="false" max="25" min="24" style="5" width="5.1921568627451"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="5" width="4.57647058823529"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="5" width="4.41176470588235"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="5" width="4.88235294117647"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="5" width="4.10588235294118"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="5" width="4.24313725490196"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="5" width="4.72156862745098"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="5" width="3.94509803921569"/>
+    <col collapsed="false" hidden="false" max="257" min="33" style="0" width="8.72941176470588"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
@@ -1823,7 +1826,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="17.6" outlineLevel="0" r="2">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="39" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1898,7 +1901,7 @@
       <c r="AF3" s="24"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="17.6" outlineLevel="0" r="5">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="39" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1975,7 +1978,7 @@
       <c r="AF6" s="19"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="17.6" outlineLevel="0" r="8">
-      <c r="A8" s="38" t="s">
+      <c r="A8" s="39" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2054,7 +2057,7 @@
       <c r="AF9" s="7"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="17.6" outlineLevel="0" r="11">
-      <c r="A11" s="38" t="s">
+      <c r="A11" s="39" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2121,7 +2124,7 @@
       <c r="AF12" s="19"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="17.6" outlineLevel="0" r="14">
-      <c r="A14" s="38" t="s">
+      <c r="A14" s="39" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2208,7 +2211,7 @@
       <c r="AF15" s="7"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="17.6" outlineLevel="0" r="17">
-      <c r="A17" s="38" t="s">
+      <c r="A17" s="39" t="s">
         <v>22</v>
       </c>
     </row>
@@ -2269,7 +2272,7 @@
       <c r="AF18" s="7"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="17.6" outlineLevel="0" r="20">
-      <c r="A20" s="38" t="s">
+      <c r="A20" s="39" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2334,7 +2337,7 @@
       <c r="AF21" s="19"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="17.6" outlineLevel="0" r="23">
-      <c r="A23" s="38" t="s">
+      <c r="A23" s="39" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2419,7 +2422,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="17.6" outlineLevel="0" r="26">
-      <c r="A26" s="38" t="s">
+      <c r="A26" s="39" t="s">
         <v>25</v>
       </c>
     </row>
@@ -2490,7 +2493,7 @@
       <c r="AF27" s="19"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="17.6" outlineLevel="0" r="29">
-      <c r="A29" s="38" t="s">
+      <c r="A29" s="39" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2565,7 +2568,7 @@
       <c r="AF30" s="24"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="17.6" outlineLevel="0" r="32">
-      <c r="A32" s="38" t="s">
+      <c r="A32" s="39" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2704,7 +2707,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="17.6" outlineLevel="0" r="38">
-      <c r="A38" s="38" t="s">
+      <c r="A38" s="39" t="s">
         <v>17</v>
       </c>
     </row>
@@ -3577,7 +3580,7 @@
       <c r="S64" s="27"/>
       <c r="T64" s="27"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.25" outlineLevel="0" r="65">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="65">
       <c r="A65" s="25"/>
       <c r="B65" s="7"/>
       <c r="C65" s="10"/>
@@ -3649,44 +3652,40 @@
   </sheetPr>
   <dimension ref="A1:AF69"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="true" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <pane activePane="bottomRight" topLeftCell="B29" xSplit="1" ySplit="1"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
-      <selection activeCell="B1" activeCellId="0" pane="topRight" sqref="B1"/>
-      <selection activeCell="A29" activeCellId="0" pane="bottomLeft" sqref="A29"/>
-      <selection activeCell="J39" activeCellId="0" pane="bottomRight" sqref="J39"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.5254901960784"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="5.45490196078431"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="6.37647058823529"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="5.6078431372549"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="5" width="5.75294117647059"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="5.45490196078431"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="5" width="5.75294117647059"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="5" width="5.90588235294118"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="5" width="5.75294117647059"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="5" width="5.16470588235294"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="5" width="5.75294117647059"/>
-    <col collapsed="false" hidden="false" max="16" min="13" style="5" width="5.6078431372549"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="5" width="5.75294117647059"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="5" width="4.85490196078431"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="5" width="5.16470588235294"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="5" width="6.05882352941176"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="5" width="5.90588235294118"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="5" width="5.53333333333333"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="5" width="5.69019607843137"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="5" width="5.37254901960784"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="5" width="5.84313725490196"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="5" width="5.37254901960784"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="5" width="6.05882352941176"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="5" width="4.85490196078431"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="5" width="4.54901960784314"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="5" width="4.38823529411765"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="5" width="4.85490196078431"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="5" width="5.01176470588235"/>
-    <col collapsed="false" hidden="false" max="257" min="33" style="0" width="8.68235294117647"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.6039215686275"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="5.48235294117647"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="6.41176470588235"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="5.63529411764706"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="5" width="5.78039215686275"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="5.48235294117647"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="5" width="5.78039215686275"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="5" width="5.94117647058824"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="5" width="5.78039215686275"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="5" width="5.1921568627451"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="5" width="5.78039215686275"/>
+    <col collapsed="false" hidden="false" max="16" min="13" style="5" width="5.63529411764706"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="5" width="5.78039215686275"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="5" width="4.88235294117647"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="5" width="5.1921568627451"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="5" width="6.09411764705882"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="5" width="5.94117647058824"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="5" width="5.56078431372549"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="5" width="5.71764705882353"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="5" width="5.4"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="5" width="5.87058823529412"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="5" width="5.4"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="5" width="6.09411764705882"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="5" width="4.88235294117647"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="5" width="4.57647058823529"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="5" width="4.41176470588235"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="5" width="4.88235294117647"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="5" width="5.03921568627451"/>
+    <col collapsed="false" hidden="false" max="257" min="33" style="0" width="8.72941176470588"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
@@ -5561,7 +5560,7 @@
       <c r="S68" s="27"/>
       <c r="T68" s="27"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.25" outlineLevel="0" r="69">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="69">
       <c r="A69" s="25"/>
       <c r="B69" s="11"/>
       <c r="C69" s="13" t="n">
@@ -5633,42 +5632,42 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AF54"/>
+  <dimension ref="A1:AF69"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2"/>
+      <selection activeCell="AE3" activeCellId="0" pane="topLeft" sqref="AE3:AF3"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.4156862745098"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="5.01176470588235"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="5" width="5.75294117647059"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="6.55686274509804"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="5" width="5.45490196078431"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="5" width="5.16470588235294"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="5" width="4.85490196078431"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="5" width="5.45490196078431"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="5" width="5.16470588235294"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="5" width="4.69411764705882"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="5" width="5.01176470588235"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="5" width="4.85490196078431"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="5" width="5.90588235294118"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="5" width="5.45490196078431"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="5" width="5.75294117647059"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="5" width="5.90588235294118"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="5" width="6.37647058823529"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="5" width="5.90588235294118"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="5" width="5.6078431372549"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="5" width="5.75294117647059"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="5" width="5.31764705882353"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="5" width="5.16470588235294"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="5" width="5.31764705882353"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="5" width="5.45490196078431"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="5" width="5.01176470588235"/>
-    <col collapsed="false" hidden="false" max="30" min="28" style="5" width="5.31764705882353"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="5" width="4.54901960784314"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="5" width="5.90588235294118"/>
-    <col collapsed="false" hidden="false" max="257" min="33" style="0" width="8.68235294117647"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.4901960784314"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="5.03921568627451"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="5" width="5.78039215686275"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="6.5921568627451"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="5" width="5.48235294117647"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="5" width="5.1921568627451"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="5" width="4.88235294117647"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="5" width="5.48235294117647"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="5" width="5.1921568627451"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="5" width="4.72156862745098"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="5" width="5.03921568627451"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="5" width="4.88235294117647"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="5" width="5.94117647058824"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="5" width="5.48235294117647"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="5" width="5.78039215686275"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="5" width="5.94117647058824"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="5" width="6.41176470588235"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="5" width="5.94117647058824"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="5" width="5.63529411764706"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="5" width="5.78039215686275"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="5" width="5.34509803921569"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="5" width="5.1921568627451"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="5" width="5.34509803921569"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="5" width="5.48235294117647"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="5" width="5.03921568627451"/>
+    <col collapsed="false" hidden="false" max="30" min="28" style="5" width="5.34509803921569"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="5" width="4.57647058823529"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="5" width="5.94117647058824"/>
+    <col collapsed="false" hidden="false" max="257" min="33" style="0" width="8.72941176470588"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
@@ -5766,9 +5765,48 @@
         <v>31</v>
       </c>
     </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="17.6" outlineLevel="0" r="2">
+      <c r="A2" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="3">
+      <c r="A3" s="28"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="10"/>
+      <c r="R3" s="10"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="10"/>
+      <c r="U3" s="10"/>
+      <c r="V3" s="10"/>
+      <c r="W3" s="10"/>
+      <c r="X3" s="10"/>
+      <c r="Y3" s="10"/>
+      <c r="Z3" s="10"/>
+      <c r="AA3" s="10"/>
+      <c r="AB3" s="10"/>
+      <c r="AC3" s="10"/>
+      <c r="AD3" s="10"/>
+      <c r="AE3" s="29"/>
+      <c r="AF3" s="29"/>
+    </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="17.6" outlineLevel="0" r="5">
       <c r="A5" s="2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.25" outlineLevel="0" r="6">
@@ -5776,18 +5814,14 @@
       <c r="B6" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="C6" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10" t="n">
-        <v>1</v>
-      </c>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="H6" s="10"/>
       <c r="I6" s="10" t="n">
         <v>1</v>
       </c>
@@ -5801,47 +5835,43 @@
       <c r="M6" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="N6" s="10"/>
-      <c r="O6" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="P6" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q6" s="10"/>
-      <c r="R6" s="10"/>
-      <c r="S6" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="T6" s="10"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="13"/>
+      <c r="P6" s="13"/>
+      <c r="Q6" s="13"/>
+      <c r="R6" s="13"/>
+      <c r="S6" s="13" t="n">
+        <v>6</v>
+      </c>
+      <c r="T6" s="13" t="n">
+        <v>7</v>
+      </c>
       <c r="U6" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="V6" s="9"/>
-      <c r="W6" s="9"/>
-      <c r="X6" s="9"/>
-      <c r="Y6" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="Z6" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA6" s="10"/>
-      <c r="AB6" s="10"/>
-      <c r="AC6" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD6" s="10"/>
+      <c r="V6" s="10"/>
+      <c r="W6" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="X6" s="14"/>
+      <c r="Y6" s="14"/>
+      <c r="Z6" s="14"/>
+      <c r="AA6" s="14"/>
+      <c r="AB6" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC6" s="10"/>
+      <c r="AD6" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="AE6" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="AF6" s="10" t="n">
-        <v>1</v>
-      </c>
+      <c r="AF6" s="10"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="17.6" outlineLevel="0" r="8">
       <c r="A8" s="2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.25" outlineLevel="0" r="9">
@@ -5853,41 +5883,47 @@
       <c r="D9" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="10" t="n">
-        <v>1</v>
-      </c>
+      <c r="E9" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="H9" s="10"/>
       <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
+      <c r="J9" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="K9" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="L9" s="9"/>
-      <c r="M9" s="9"/>
-      <c r="N9" s="9"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="N9" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="O9" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="P9" s="10"/>
-      <c r="Q9" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="R9" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="S9" s="10"/>
-      <c r="T9" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="U9" s="10"/>
-      <c r="V9" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="W9" s="9"/>
-      <c r="X9" s="9"/>
-      <c r="Y9" s="9"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="9"/>
+      <c r="R9" s="9"/>
+      <c r="S9" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="T9" s="14"/>
+      <c r="U9" s="14"/>
+      <c r="V9" s="14"/>
+      <c r="W9" s="14"/>
+      <c r="X9" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y9" s="10"/>
       <c r="Z9" s="10" t="n">
         <v>1</v>
       </c>
@@ -5895,74 +5931,73 @@
       <c r="AB9" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="AC9" s="13"/>
-      <c r="AD9" s="13"/>
-      <c r="AE9" s="13"/>
+      <c r="AC9" s="9"/>
+      <c r="AD9" s="9"/>
+      <c r="AE9" s="9"/>
+      <c r="AF9" s="29"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="17.6" outlineLevel="0" r="11">
       <c r="A11" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.25" outlineLevel="0" r="12">
       <c r="A12" s="28"/>
-      <c r="B12" s="13" t="n">
-        <v>4</v>
-      </c>
-      <c r="C12" s="13" t="n">
-        <v>5</v>
-      </c>
+      <c r="B12" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" s="10"/>
       <c r="D12" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
       <c r="I12" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="J12" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="K12" s="10"/>
-      <c r="L12" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="M12" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="N12" s="10"/>
-      <c r="O12" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="P12" s="10"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="13"/>
+      <c r="N12" s="13"/>
+      <c r="O12" s="13" t="n">
+        <v>6</v>
+      </c>
+      <c r="P12" s="13" t="n">
+        <v>7</v>
+      </c>
       <c r="Q12" s="10" t="n">
         <v>1</v>
       </c>
       <c r="R12" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="S12" s="13"/>
-      <c r="T12" s="13"/>
-      <c r="U12" s="13"/>
-      <c r="V12" s="13"/>
-      <c r="W12" s="13"/>
-      <c r="X12" s="13"/>
-      <c r="Y12" s="13"/>
-      <c r="Z12" s="13" t="n">
-        <v>8</v>
-      </c>
-      <c r="AA12" s="13" t="n">
-        <v>9</v>
-      </c>
-      <c r="AB12" s="13" t="n">
-        <v>10</v>
-      </c>
+      <c r="S12" s="10"/>
+      <c r="T12" s="10"/>
+      <c r="U12" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="V12" s="10"/>
+      <c r="W12" s="10"/>
+      <c r="X12" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y12" s="10"/>
+      <c r="Z12" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA12" s="10"/>
+      <c r="AB12" s="10"/>
       <c r="AC12" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="AD12" s="10"/>
+      <c r="AD12" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="AE12" s="10" t="n">
         <v>1</v>
       </c>
@@ -5970,30 +6005,30 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="17.6" outlineLevel="0" r="14">
       <c r="A14" s="2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.25" outlineLevel="0" r="15">
       <c r="A15" s="28"/>
-      <c r="B15" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="M15" s="10" t="n">
-        <v>1</v>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13" t="n">
+        <v>6</v>
+      </c>
+      <c r="M15" s="13" t="n">
+        <v>7</v>
       </c>
       <c r="N15" s="10" t="n">
         <v>1</v>
@@ -6001,46 +6036,46 @@
       <c r="O15" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="P15" s="10"/>
+      <c r="P15" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="Q15" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="R15" s="10"/>
-      <c r="S15" s="10"/>
-      <c r="T15" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="U15" s="10"/>
+      <c r="R15" s="14"/>
+      <c r="S15" s="14"/>
+      <c r="T15" s="14"/>
+      <c r="U15" s="14"/>
       <c r="V15" s="10" t="n">
         <v>1</v>
       </c>
       <c r="W15" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="X15" s="10"/>
-      <c r="Y15" s="10"/>
-      <c r="Z15" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA15" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB15" s="10"/>
-      <c r="AC15" s="10"/>
-      <c r="AD15" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="AE15" s="10"/>
+      <c r="X15" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y15" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z15" s="9"/>
+      <c r="AA15" s="9"/>
+      <c r="AB15" s="9"/>
+      <c r="AC15" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD15" s="9"/>
+      <c r="AE15" s="9"/>
       <c r="AF15" s="29"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="17.6" outlineLevel="0" r="17">
       <c r="A17" s="2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.25" outlineLevel="0" r="18">
       <c r="A18" s="28"/>
-      <c r="B18" s="10"/>
+      <c r="B18" s="9"/>
       <c r="C18" s="10" t="n">
         <v>1</v>
       </c>
@@ -6049,130 +6084,138 @@
       <c r="F18" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="I18" s="13"/>
-      <c r="J18" s="13" t="n">
+      <c r="J18" s="13"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="K18" s="13" t="n">
+      <c r="M18" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="L18" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="M18" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="N18" s="10"/>
-      <c r="O18" s="10" t="n">
-        <v>1</v>
-      </c>
+      <c r="N18" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="O18" s="10"/>
       <c r="P18" s="10"/>
       <c r="Q18" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="R18" s="10"/>
-      <c r="S18" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="T18" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="U18" s="14"/>
-      <c r="V18" s="14"/>
-      <c r="W18" s="14"/>
-      <c r="X18" s="14"/>
-      <c r="Y18" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="Z18" s="10"/>
-      <c r="AA18" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB18" s="10"/>
-      <c r="AC18" s="10"/>
-      <c r="AD18" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="AE18" s="10"/>
+      <c r="R18" s="13"/>
+      <c r="S18" s="13"/>
+      <c r="T18" s="13"/>
+      <c r="U18" s="13" t="n">
+        <v>4</v>
+      </c>
+      <c r="V18" s="13" t="n">
+        <v>5</v>
+      </c>
+      <c r="W18" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="X18" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y18" s="13"/>
+      <c r="Z18" s="13"/>
+      <c r="AA18" s="13"/>
+      <c r="AB18" s="13"/>
+      <c r="AC18" s="13" t="n">
+        <v>5</v>
+      </c>
+      <c r="AD18" s="13" t="n">
+        <v>6</v>
+      </c>
+      <c r="AE18" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="AF18" s="10" t="n">
         <v>1</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="17.6" outlineLevel="0" r="20">
       <c r="A20" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.25" outlineLevel="0" r="21">
+        <v>22</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="21">
       <c r="A21" s="28"/>
       <c r="B21" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="10" t="n">
-        <v>1</v>
-      </c>
+      <c r="C21" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="F21" s="10"/>
       <c r="G21" s="10"/>
       <c r="H21" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="I21" s="10"/>
+      <c r="I21" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="J21" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="K21" s="13"/>
-      <c r="L21" s="13"/>
-      <c r="M21" s="13"/>
-      <c r="N21" s="13" t="n">
-        <v>4</v>
-      </c>
-      <c r="O21" s="13" t="n">
-        <v>5</v>
+      <c r="K21" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L21" s="10"/>
+      <c r="M21" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="N21" s="10"/>
+      <c r="O21" s="10" t="n">
+        <v>1</v>
       </c>
       <c r="P21" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="Q21" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="R21" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="S21" s="9"/>
-      <c r="T21" s="9"/>
-      <c r="U21" s="9"/>
-      <c r="V21" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="W21" s="10" t="n">
-        <v>1</v>
-      </c>
+      <c r="Q21" s="10"/>
+      <c r="R21" s="10"/>
+      <c r="S21" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="T21" s="10"/>
+      <c r="U21" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="V21" s="9"/>
+      <c r="W21" s="9"/>
       <c r="X21" s="9"/>
-      <c r="Y21" s="9"/>
-      <c r="Z21" s="9"/>
-      <c r="AA21" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB21" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC21" s="10"/>
+      <c r="Y21" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z21" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA21" s="10"/>
+      <c r="AB21" s="10"/>
+      <c r="AC21" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="AD21" s="10"/>
       <c r="AE21" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="AF21" s="10"/>
+      <c r="AF21" s="10" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="17.6" outlineLevel="0" r="23">
       <c r="A23" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.25" outlineLevel="0" r="24">
+        <v>23</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="24">
       <c r="A24" s="28"/>
       <c r="B24" s="10" t="n">
         <v>1</v>
@@ -6181,522 +6224,464 @@
       <c r="D24" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13" t="n">
-        <v>4</v>
-      </c>
-      <c r="I24" s="13" t="n">
-        <v>5</v>
-      </c>
-      <c r="J24" s="19"/>
-      <c r="K24" s="19"/>
-      <c r="L24" s="19"/>
-      <c r="M24" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="N24" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="O24" s="30" t="s">
-        <v>30</v>
-      </c>
-      <c r="P24" s="30"/>
-      <c r="Q24" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="R24" s="30" t="s">
-        <v>30</v>
-      </c>
-      <c r="S24" s="30"/>
-      <c r="T24" s="10"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="I24" s="10"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L24" s="9"/>
+      <c r="M24" s="9"/>
+      <c r="N24" s="9"/>
+      <c r="O24" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="P24" s="10"/>
+      <c r="Q24" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="R24" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="S24" s="10"/>
+      <c r="T24" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="U24" s="10"/>
       <c r="V24" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="W24" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="X24" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="Y24" s="10"/>
-      <c r="Z24" s="10"/>
-      <c r="AA24" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB24" s="10"/>
-      <c r="AC24" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD24" s="29"/>
-      <c r="AE24" s="29"/>
+      <c r="W24" s="9"/>
+      <c r="X24" s="9"/>
+      <c r="Y24" s="9"/>
+      <c r="Z24" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA24" s="10"/>
+      <c r="AB24" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC24" s="13"/>
+      <c r="AD24" s="13"/>
+      <c r="AE24" s="13"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="17.6" outlineLevel="0" r="26">
       <c r="A26" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.25" outlineLevel="0" r="27">
+        <v>24</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="27">
       <c r="A27" s="28"/>
-      <c r="B27" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="C27" s="10" t="n">
-        <v>1</v>
+      <c r="B27" s="13" t="n">
+        <v>4</v>
+      </c>
+      <c r="C27" s="13" t="n">
+        <v>5</v>
       </c>
       <c r="D27" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="G27" s="9"/>
-      <c r="H27" s="9"/>
-      <c r="I27" s="9"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="14"/>
+      <c r="I27" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="J27" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="K27" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="L27" s="13"/>
-      <c r="M27" s="13"/>
-      <c r="N27" s="13"/>
-      <c r="O27" s="13" t="n">
-        <v>4</v>
-      </c>
-      <c r="P27" s="13" t="n">
-        <v>5</v>
-      </c>
+      <c r="K27" s="10"/>
+      <c r="L27" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="M27" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="N27" s="10"/>
+      <c r="O27" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="P27" s="10"/>
       <c r="Q27" s="10" t="n">
         <v>1</v>
       </c>
       <c r="R27" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="S27" s="10"/>
-      <c r="T27" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="U27" s="10"/>
-      <c r="V27" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="W27" s="9"/>
-      <c r="X27" s="9"/>
-      <c r="Y27" s="9"/>
-      <c r="Z27" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA27" s="13"/>
-      <c r="AB27" s="13"/>
-      <c r="AC27" s="13"/>
-      <c r="AD27" s="13" t="n">
-        <v>4</v>
-      </c>
-      <c r="AE27" s="13" t="n">
-        <v>5</v>
-      </c>
-      <c r="AF27" s="10" t="n">
-        <v>1</v>
-      </c>
+      <c r="S27" s="13"/>
+      <c r="T27" s="13"/>
+      <c r="U27" s="13"/>
+      <c r="V27" s="13"/>
+      <c r="W27" s="13"/>
+      <c r="X27" s="13"/>
+      <c r="Y27" s="13"/>
+      <c r="Z27" s="13" t="n">
+        <v>8</v>
+      </c>
+      <c r="AA27" s="13" t="n">
+        <v>9</v>
+      </c>
+      <c r="AB27" s="13" t="n">
+        <v>10</v>
+      </c>
+      <c r="AC27" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD27" s="10"/>
+      <c r="AE27" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF27" s="10"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="17.6" outlineLevel="0" r="29">
       <c r="A29" s="2" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="30">
-      <c r="A30" s="6"/>
-      <c r="B30" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="E30" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="F30" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="G30" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H30" s="8"/>
-      <c r="I30" s="8"/>
-      <c r="J30" s="8"/>
-      <c r="K30" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="L30" s="8"/>
-      <c r="M30" s="8"/>
-      <c r="N30" s="8"/>
-      <c r="O30" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="P30" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q30" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="R30" s="7"/>
-      <c r="S30" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="T30" s="7"/>
-      <c r="U30" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="V30" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="W30" s="13"/>
-      <c r="X30" s="13"/>
-      <c r="Y30" s="13"/>
-      <c r="Z30" s="13"/>
-      <c r="AA30" s="13"/>
-      <c r="AB30" s="13" t="n">
-        <v>6</v>
-      </c>
-      <c r="AC30" s="13" t="n">
-        <v>7</v>
-      </c>
-      <c r="AD30" s="13" t="n">
-        <v>8</v>
-      </c>
-      <c r="AE30" s="13" t="n">
-        <v>9</v>
-      </c>
-      <c r="AF30" s="19"/>
+      <c r="A30" s="28"/>
+      <c r="B30" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C30" s="14"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
+      <c r="G30" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="H30" s="14"/>
+      <c r="I30" s="14"/>
+      <c r="J30" s="14"/>
+      <c r="K30" s="14"/>
+      <c r="L30" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="M30" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="N30" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="O30" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="P30" s="10"/>
+      <c r="Q30" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="R30" s="10"/>
+      <c r="S30" s="10"/>
+      <c r="T30" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="U30" s="10"/>
+      <c r="V30" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="W30" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="X30" s="10"/>
+      <c r="Y30" s="10"/>
+      <c r="Z30" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA30" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB30" s="10"/>
+      <c r="AC30" s="10"/>
+      <c r="AD30" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE30" s="10"/>
+      <c r="AF30" s="30"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="17.6" outlineLevel="0" r="32">
       <c r="A32" s="2" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="33">
-      <c r="A33" s="6"/>
-      <c r="B33" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H33" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="I33" s="7"/>
-      <c r="J33" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="K33" s="8"/>
-      <c r="L33" s="8"/>
-      <c r="M33" s="8"/>
-      <c r="N33" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="O33" s="7"/>
-      <c r="P33" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q33" s="7"/>
-      <c r="R33" s="7"/>
-      <c r="S33" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="T33" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="U33" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="V33" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="W33" s="7"/>
-      <c r="X33" s="7"/>
-      <c r="Y33" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="Z33" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA33" s="13"/>
-      <c r="AB33" s="13"/>
-      <c r="AC33" s="13"/>
-      <c r="AD33" s="13" t="n">
+      <c r="A33" s="28"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="G33" s="13"/>
+      <c r="H33" s="13"/>
+      <c r="I33" s="13"/>
+      <c r="J33" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="AE33" s="13" t="n">
+      <c r="K33" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="AF33" s="7" t="n">
+      <c r="L33" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="M33" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="N33" s="10"/>
+      <c r="O33" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="P33" s="10"/>
+      <c r="Q33" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="R33" s="10"/>
+      <c r="S33" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="T33" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="U33" s="14"/>
+      <c r="V33" s="14"/>
+      <c r="W33" s="14"/>
+      <c r="X33" s="14"/>
+      <c r="Y33" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z33" s="10"/>
+      <c r="AA33" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB33" s="10"/>
+      <c r="AC33" s="10"/>
+      <c r="AD33" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE33" s="10"/>
+      <c r="AF33" s="10" t="n">
         <v>1</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="17.6" outlineLevel="0" r="35">
       <c r="A35" s="2" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="36">
-      <c r="A36" s="6"/>
-      <c r="B36" s="7"/>
-      <c r="C36" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D36" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="E36" s="8"/>
-      <c r="F36" s="8"/>
-      <c r="G36" s="8"/>
-      <c r="H36" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="I36" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="J36" s="7"/>
-      <c r="K36" s="7"/>
-      <c r="L36" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="M36" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="N36" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="O36" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="P36" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q36" s="13" t="n">
+      <c r="A36" s="28"/>
+      <c r="B36" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="G36" s="10"/>
+      <c r="H36" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="I36" s="10"/>
+      <c r="J36" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="K36" s="13"/>
+      <c r="L36" s="13"/>
+      <c r="M36" s="13"/>
+      <c r="N36" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="R36" s="13" t="n">
+      <c r="O36" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="S36" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="T36" s="7"/>
-      <c r="U36" s="7"/>
-      <c r="V36" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="W36" s="7"/>
-      <c r="X36" s="7"/>
-      <c r="Y36" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="Z36" s="7"/>
-      <c r="AA36" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="AB36" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="AC36" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="AD36" s="13" t="n">
-        <v>4</v>
-      </c>
-      <c r="AE36" s="13" t="n">
-        <v>5</v>
-      </c>
-      <c r="AF36" s="19"/>
+      <c r="P36" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q36" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="R36" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="S36" s="9"/>
+      <c r="T36" s="9"/>
+      <c r="U36" s="9"/>
+      <c r="V36" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="W36" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="X36" s="9"/>
+      <c r="Y36" s="9"/>
+      <c r="Z36" s="9"/>
+      <c r="AA36" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB36" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC36" s="10"/>
+      <c r="AD36" s="10"/>
+      <c r="AE36" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF36" s="10"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="17.6" outlineLevel="0" r="38">
       <c r="A38" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="39">
-      <c r="A39" s="6"/>
-      <c r="B39" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="C39" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="D39" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="E39" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="F39" s="8"/>
-      <c r="G39" s="8"/>
-      <c r="H39" s="8"/>
-      <c r="I39" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="J39" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="K39" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="L39" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="M39" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="N39" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="O39" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="P39" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q39" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="R39" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="S39" s="13" t="n">
-        <v>10</v>
-      </c>
-      <c r="T39" s="13" t="n">
-        <v>11</v>
-      </c>
-      <c r="U39" s="13" t="n">
-        <v>12</v>
-      </c>
-      <c r="V39" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="W39" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="X39" s="7"/>
-      <c r="Y39" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="Z39" s="7"/>
-      <c r="AA39" s="7"/>
-      <c r="AB39" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC39" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD39" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="AE39" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="AF39" s="7" t="n">
-        <v>1</v>
-      </c>
+        <v>16</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.25" outlineLevel="0" r="39">
+      <c r="A39" s="28"/>
+      <c r="B39" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E39" s="13"/>
+      <c r="F39" s="13"/>
+      <c r="G39" s="13"/>
+      <c r="H39" s="13" t="n">
+        <v>4</v>
+      </c>
+      <c r="I39" s="13" t="n">
+        <v>5</v>
+      </c>
+      <c r="J39" s="19"/>
+      <c r="K39" s="19"/>
+      <c r="L39" s="19"/>
+      <c r="M39" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="N39" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="O39" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="P39" s="31"/>
+      <c r="Q39" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="R39" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="S39" s="31"/>
+      <c r="T39" s="10"/>
+      <c r="U39" s="10"/>
+      <c r="V39" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="W39" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="X39" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y39" s="10"/>
+      <c r="Z39" s="10"/>
+      <c r="AA39" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB39" s="10"/>
+      <c r="AC39" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD39" s="30"/>
+      <c r="AE39" s="30"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="17.6" outlineLevel="0" r="41">
       <c r="A41" s="2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="42">
-      <c r="A42" s="25"/>
-      <c r="B42" s="7"/>
-      <c r="C42" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D42" s="7"/>
-      <c r="E42" s="7"/>
-      <c r="F42" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="G42" s="7"/>
-      <c r="H42" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="I42" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="J42" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="K42" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="L42" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="M42" s="13" t="n">
+      <c r="A42" s="28"/>
+      <c r="B42" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C42" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D42" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E42" s="10"/>
+      <c r="F42" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="G42" s="9"/>
+      <c r="H42" s="9"/>
+      <c r="I42" s="9"/>
+      <c r="J42" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="K42" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L42" s="13"/>
+      <c r="M42" s="13"/>
+      <c r="N42" s="13"/>
+      <c r="O42" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="N42" s="13" t="n">
+      <c r="P42" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="O42" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="P42" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q42" s="7"/>
-      <c r="R42" s="7"/>
-      <c r="S42" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="T42" s="7"/>
-      <c r="U42" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="V42" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="W42" s="7"/>
-      <c r="X42" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="Y42" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="Z42" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA42" s="7"/>
-      <c r="AB42" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC42" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD42" s="10"/>
-      <c r="AE42" s="10"/>
-      <c r="AF42" s="7"/>
+      <c r="Q42" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="R42" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="S42" s="10"/>
+      <c r="T42" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="U42" s="10"/>
+      <c r="V42" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="W42" s="9"/>
+      <c r="X42" s="9"/>
+      <c r="Y42" s="9"/>
+      <c r="Z42" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA42" s="13"/>
+      <c r="AB42" s="13"/>
+      <c r="AC42" s="13"/>
+      <c r="AD42" s="13" t="n">
+        <v>4</v>
+      </c>
+      <c r="AE42" s="13" t="n">
+        <v>5</v>
+      </c>
+      <c r="AF42" s="10" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="17.6" outlineLevel="0" r="44">
       <c r="A44" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="AF44" s="26"/>
+        <v>18</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="45">
-      <c r="A45" s="25"/>
+      <c r="A45" s="6"/>
       <c r="B45" s="7" t="n">
         <v>1</v>
       </c>
@@ -6704,138 +6689,92 @@
       <c r="D45" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="E45" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="F45" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="G45" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="H45" s="13" t="n">
-        <v>4</v>
-      </c>
-      <c r="I45" s="13" t="n">
-        <v>5</v>
-      </c>
-      <c r="J45" s="7" t="n">
-        <v>1</v>
-      </c>
+      <c r="E45" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F45" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G45" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="H45" s="8"/>
+      <c r="I45" s="8"/>
+      <c r="J45" s="8"/>
       <c r="K45" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="L45" s="7"/>
-      <c r="M45" s="7"/>
-      <c r="N45" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="O45" s="7"/>
+      <c r="L45" s="8"/>
+      <c r="M45" s="8"/>
+      <c r="N45" s="8"/>
+      <c r="O45" s="7" t="n">
+        <v>1</v>
+      </c>
       <c r="P45" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="Q45" s="7"/>
+      <c r="Q45" s="7" t="n">
+        <v>1</v>
+      </c>
       <c r="R45" s="7"/>
       <c r="S45" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="T45" s="7" t="n">
-        <v>1</v>
-      </c>
+      <c r="T45" s="7"/>
       <c r="U45" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="V45" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="W45" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="X45" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="Y45" s="13" t="n">
-        <v>4</v>
-      </c>
-      <c r="Z45" s="13" t="n">
-        <v>5</v>
-      </c>
-      <c r="AA45" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB45" s="7"/>
-      <c r="AC45" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD45" s="7"/>
-      <c r="AE45" s="7"/>
+      <c r="V45" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="W45" s="13"/>
+      <c r="X45" s="13"/>
+      <c r="Y45" s="13"/>
+      <c r="Z45" s="13"/>
+      <c r="AA45" s="13"/>
+      <c r="AB45" s="13" t="n">
+        <v>6</v>
+      </c>
+      <c r="AC45" s="13" t="n">
+        <v>7</v>
+      </c>
+      <c r="AD45" s="13" t="n">
+        <v>8</v>
+      </c>
+      <c r="AE45" s="13" t="n">
+        <v>9</v>
+      </c>
       <c r="AF45" s="19"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="17.6" outlineLevel="0" r="47">
       <c r="A47" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="S47" s="27"/>
-      <c r="T47" s="27" t="n">
-        <v>12</v>
-      </c>
-      <c r="Y47" s="5" t="n">
-        <v>44</v>
-      </c>
-      <c r="Z47" s="5" t="n">
-        <v>24</v>
-      </c>
-      <c r="AA47" s="5" t="n">
-        <v>26</v>
-      </c>
-      <c r="AB47" s="5" t="n">
-        <v>14</v>
-      </c>
-      <c r="AC47" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="AD47" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="AE47" s="5" t="n">
-        <v>16</v>
-      </c>
-      <c r="AF47" s="5" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="48">
-      <c r="A48" s="25"/>
+      <c r="A48" s="6"/>
       <c r="B48" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="C48" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D48" s="7"/>
-      <c r="E48" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="F48" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="G48" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="H48" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="I48" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="J48" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="K48" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="L48" s="7"/>
-      <c r="M48" s="7"/>
+      <c r="C48" s="7"/>
+      <c r="D48" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E48" s="7"/>
+      <c r="F48" s="7"/>
+      <c r="G48" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="H48" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="I48" s="7"/>
+      <c r="J48" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K48" s="8"/>
+      <c r="L48" s="8"/>
+      <c r="M48" s="8"/>
       <c r="N48" s="7" t="n">
         <v>1</v>
       </c>
@@ -6843,309 +6782,741 @@
       <c r="P48" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="Q48" s="8"/>
-      <c r="R48" s="8"/>
-      <c r="S48" s="8"/>
+      <c r="Q48" s="7"/>
+      <c r="R48" s="7"/>
+      <c r="S48" s="7" t="n">
+        <v>1</v>
+      </c>
       <c r="T48" s="7" t="n">
         <v>1</v>
       </c>
       <c r="U48" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="V48" s="8"/>
-      <c r="W48" s="8"/>
-      <c r="X48" s="8"/>
+      <c r="V48" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="W48" s="7"/>
+      <c r="X48" s="7"/>
       <c r="Y48" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="Z48" s="24"/>
-      <c r="AA48" s="24"/>
-      <c r="AB48" s="24"/>
-      <c r="AC48" s="24"/>
-      <c r="AD48" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="AE48" s="8"/>
-      <c r="AF48" s="8"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="49">
-      <c r="A49" s="3"/>
+      <c r="Z48" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA48" s="13"/>
+      <c r="AB48" s="13"/>
+      <c r="AC48" s="13"/>
+      <c r="AD48" s="13" t="n">
+        <v>4</v>
+      </c>
+      <c r="AE48" s="13" t="n">
+        <v>5</v>
+      </c>
+      <c r="AF48" s="7" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="17.6" outlineLevel="0" r="50">
       <c r="A50" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B50" s="5" t="n">
-        <v>11</v>
-      </c>
-      <c r="C50" s="5" t="n">
-        <v>21</v>
-      </c>
-      <c r="D50" s="5" t="n">
-        <v>16</v>
-      </c>
-      <c r="E50" s="5" t="n">
         <v>20</v>
       </c>
-      <c r="F50" s="5" t="n">
-        <v>20</v>
-      </c>
-      <c r="G50" s="5" t="n">
-        <v>24</v>
-      </c>
-      <c r="H50" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="I50" s="5" t="n">
-        <v>11</v>
-      </c>
-      <c r="J50" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="K50" s="5" t="n">
-        <v>33</v>
-      </c>
-      <c r="L50" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="M50" s="5" t="n">
-        <v>17</v>
-      </c>
-      <c r="N50" s="5" t="n">
-        <v>15</v>
-      </c>
-      <c r="O50" s="5" t="n">
-        <v>17</v>
-      </c>
-      <c r="P50" s="5" t="n">
-        <v>13</v>
-      </c>
-      <c r="Q50" s="5" t="n">
-        <v>10</v>
-      </c>
-      <c r="R50" s="5" t="n">
-        <v>16</v>
-      </c>
-      <c r="S50" s="27" t="n">
-        <v>53</v>
-      </c>
-      <c r="T50" s="5" t="n">
-        <v>34</v>
-      </c>
-      <c r="U50" s="27" t="n">
-        <v>10</v>
-      </c>
-      <c r="V50" s="27" t="n">
-        <v>22</v>
-      </c>
-      <c r="W50" s="5" t="n">
-        <v>16</v>
-      </c>
-      <c r="X50" s="5" t="n">
-        <v>16</v>
-      </c>
-      <c r="Y50" s="5" t="n">
-        <v>56</v>
-      </c>
-      <c r="Z50" s="5" t="n">
-        <v>24</v>
-      </c>
-      <c r="AA50" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB50" s="5" t="n">
-        <v>17</v>
-      </c>
-      <c r="AC50" s="5" t="n">
-        <v>19</v>
-      </c>
-      <c r="AD50" s="5" t="n">
-        <v>11</v>
-      </c>
-      <c r="AE50" s="5" t="s">
-        <v>41</v>
-      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="51">
-      <c r="A51" s="25"/>
-      <c r="B51" s="8"/>
+      <c r="A51" s="6"/>
+      <c r="B51" s="7"/>
       <c r="C51" s="7" t="n">
         <v>1</v>
       </c>
       <c r="D51" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="E51" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="F51" s="13"/>
-      <c r="G51" s="13"/>
-      <c r="H51" s="13"/>
-      <c r="I51" s="13"/>
-      <c r="J51" s="13" t="n">
+      <c r="E51" s="8"/>
+      <c r="F51" s="8"/>
+      <c r="G51" s="8"/>
+      <c r="H51" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="I51" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="J51" s="7"/>
+      <c r="K51" s="7"/>
+      <c r="L51" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="M51" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="N51" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="O51" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="P51" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q51" s="13" t="n">
+        <v>4</v>
+      </c>
+      <c r="R51" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="K51" s="13" t="n">
-        <v>6</v>
-      </c>
-      <c r="L51" s="13" t="n">
-        <v>7</v>
-      </c>
-      <c r="M51" s="13" t="n">
-        <v>8</v>
-      </c>
-      <c r="N51" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="O51" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="P51" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q51" s="11"/>
-      <c r="R51" s="11"/>
-      <c r="S51" s="11"/>
-      <c r="T51" s="11" t="n">
-        <v>4</v>
-      </c>
-      <c r="U51" s="11" t="n">
-        <v>5</v>
-      </c>
+      <c r="S51" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="T51" s="7"/>
+      <c r="U51" s="7"/>
       <c r="V51" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="W51" s="7" t="n">
-        <v>1</v>
-      </c>
+      <c r="W51" s="7"/>
       <c r="X51" s="7"/>
       <c r="Y51" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="Z51" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="AA51" s="7"/>
-      <c r="AB51" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="AC51" s="7"/>
-      <c r="AD51" s="7"/>
-      <c r="AE51" s="7" t="n">
-        <v>1</v>
+      <c r="Z51" s="7"/>
+      <c r="AA51" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB51" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC51" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="AD51" s="13" t="n">
+        <v>4</v>
+      </c>
+      <c r="AE51" s="13" t="n">
+        <v>5</v>
       </c>
       <c r="AF51" s="19"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="17.6" outlineLevel="0" r="53">
       <c r="A53" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B53" s="5" t="n">
-        <v>14</v>
-      </c>
-      <c r="C53" s="5" t="n">
-        <v>15</v>
-      </c>
-      <c r="D53" s="5" t="n">
-        <v>28</v>
-      </c>
-      <c r="E53" s="5" t="n">
-        <v>24</v>
-      </c>
-      <c r="F53" s="5" t="n">
-        <v>38</v>
-      </c>
-      <c r="G53" s="5" t="n">
-        <v>43</v>
-      </c>
-      <c r="H53" s="5" t="n">
-        <v>13</v>
-      </c>
-      <c r="I53" s="5" t="n">
-        <v>39</v>
-      </c>
-      <c r="J53" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="K53" s="5" t="n">
-        <v>59</v>
-      </c>
-      <c r="L53" s="5" t="n">
-        <v>46</v>
-      </c>
-      <c r="M53" s="5" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="54">
+      <c r="A54" s="6"/>
+      <c r="B54" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C54" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D54" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E54" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F54" s="8"/>
+      <c r="G54" s="8"/>
+      <c r="H54" s="8"/>
+      <c r="I54" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="J54" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="K54" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="L54" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="M54" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="N54" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="O54" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="P54" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q54" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="R54" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="S54" s="13" t="n">
+        <v>10</v>
+      </c>
+      <c r="T54" s="13" t="n">
+        <v>11</v>
+      </c>
+      <c r="U54" s="13" t="n">
         <v>12</v>
       </c>
-      <c r="N53" s="5" t="n">
-        <v>13</v>
-      </c>
-      <c r="O53" s="5" t="n">
-        <v>18</v>
-      </c>
-      <c r="P53" s="5" t="n">
-        <v>43</v>
-      </c>
-      <c r="S53" s="27"/>
-      <c r="T53" s="27"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.25" outlineLevel="0" r="54">
-      <c r="A54" s="25"/>
-      <c r="B54" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C54" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="D54" s="10"/>
-      <c r="E54" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="F54" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="G54" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H54" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="I54" s="9"/>
-      <c r="J54" s="9"/>
-      <c r="K54" s="9"/>
-      <c r="L54" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="M54" s="7"/>
-      <c r="N54" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="O54" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="P54" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q54" s="7"/>
-      <c r="R54" s="7"/>
-      <c r="S54" s="7"/>
-      <c r="T54" s="7"/>
-      <c r="U54" s="7"/>
-      <c r="V54" s="7"/>
-      <c r="W54" s="7"/>
+      <c r="V54" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="W54" s="7" t="n">
+        <v>1</v>
+      </c>
       <c r="X54" s="7"/>
-      <c r="Y54" s="7"/>
+      <c r="Y54" s="7" t="n">
+        <v>1</v>
+      </c>
       <c r="Z54" s="7"/>
       <c r="AA54" s="7"/>
-      <c r="AB54" s="7"/>
-      <c r="AC54" s="7"/>
-      <c r="AD54" s="10"/>
-      <c r="AE54" s="10"/>
-      <c r="AF54" s="10"/>
+      <c r="AB54" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC54" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD54" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE54" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF54" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="17.6" outlineLevel="0" r="56">
+      <c r="A56" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="57">
+      <c r="A57" s="25"/>
+      <c r="B57" s="7"/>
+      <c r="C57" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D57" s="7"/>
+      <c r="E57" s="7"/>
+      <c r="F57" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G57" s="7"/>
+      <c r="H57" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="I57" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="J57" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="K57" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="L57" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="M57" s="13" t="n">
+        <v>4</v>
+      </c>
+      <c r="N57" s="13" t="n">
+        <v>5</v>
+      </c>
+      <c r="O57" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="P57" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q57" s="7"/>
+      <c r="R57" s="7"/>
+      <c r="S57" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="T57" s="7"/>
+      <c r="U57" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="V57" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="W57" s="7"/>
+      <c r="X57" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y57" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z57" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA57" s="7"/>
+      <c r="AB57" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC57" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD57" s="10"/>
+      <c r="AE57" s="10"/>
+      <c r="AF57" s="7"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="17.6" outlineLevel="0" r="59">
+      <c r="A59" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF59" s="26"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="60">
+      <c r="A60" s="25"/>
+      <c r="B60" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C60" s="7"/>
+      <c r="D60" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E60" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F60" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="G60" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="H60" s="13" t="n">
+        <v>4</v>
+      </c>
+      <c r="I60" s="13" t="n">
+        <v>5</v>
+      </c>
+      <c r="J60" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K60" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="L60" s="7"/>
+      <c r="M60" s="7"/>
+      <c r="N60" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="O60" s="7"/>
+      <c r="P60" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q60" s="7"/>
+      <c r="R60" s="7"/>
+      <c r="S60" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="T60" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="U60" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="V60" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="W60" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="X60" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y60" s="13" t="n">
+        <v>4</v>
+      </c>
+      <c r="Z60" s="13" t="n">
+        <v>5</v>
+      </c>
+      <c r="AA60" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB60" s="7"/>
+      <c r="AC60" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD60" s="7"/>
+      <c r="AE60" s="7"/>
+      <c r="AF60" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="17.6" outlineLevel="0" r="62">
+      <c r="A62" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S62" s="27"/>
+      <c r="T62" s="27" t="n">
+        <v>12</v>
+      </c>
+      <c r="Y62" s="5" t="n">
+        <v>44</v>
+      </c>
+      <c r="Z62" s="5" t="n">
+        <v>24</v>
+      </c>
+      <c r="AA62" s="5" t="n">
+        <v>26</v>
+      </c>
+      <c r="AB62" s="5" t="n">
+        <v>14</v>
+      </c>
+      <c r="AC62" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="AD62" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="AE62" s="5" t="n">
+        <v>16</v>
+      </c>
+      <c r="AF62" s="5" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="63">
+      <c r="A63" s="25"/>
+      <c r="B63" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C63" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D63" s="7"/>
+      <c r="E63" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F63" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G63" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="H63" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="I63" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="J63" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="K63" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="L63" s="7"/>
+      <c r="M63" s="7"/>
+      <c r="N63" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="O63" s="7"/>
+      <c r="P63" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q63" s="8"/>
+      <c r="R63" s="8"/>
+      <c r="S63" s="8"/>
+      <c r="T63" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="U63" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="V63" s="8"/>
+      <c r="W63" s="8"/>
+      <c r="X63" s="8"/>
+      <c r="Y63" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z63" s="24"/>
+      <c r="AA63" s="24"/>
+      <c r="AB63" s="24"/>
+      <c r="AC63" s="24"/>
+      <c r="AD63" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE63" s="8"/>
+      <c r="AF63" s="8"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="64">
+      <c r="A64" s="3"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="17.6" outlineLevel="0" r="65">
+      <c r="A65" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B65" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="C65" s="5" t="n">
+        <v>21</v>
+      </c>
+      <c r="D65" s="5" t="n">
+        <v>16</v>
+      </c>
+      <c r="E65" s="5" t="n">
+        <v>20</v>
+      </c>
+      <c r="F65" s="5" t="n">
+        <v>20</v>
+      </c>
+      <c r="G65" s="5" t="n">
+        <v>24</v>
+      </c>
+      <c r="H65" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I65" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="J65" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="K65" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="L65" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="M65" s="5" t="n">
+        <v>17</v>
+      </c>
+      <c r="N65" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="O65" s="5" t="n">
+        <v>17</v>
+      </c>
+      <c r="P65" s="5" t="n">
+        <v>13</v>
+      </c>
+      <c r="Q65" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="R65" s="5" t="n">
+        <v>16</v>
+      </c>
+      <c r="S65" s="27" t="n">
+        <v>53</v>
+      </c>
+      <c r="T65" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="U65" s="27" t="n">
+        <v>10</v>
+      </c>
+      <c r="V65" s="27" t="n">
+        <v>22</v>
+      </c>
+      <c r="W65" s="5" t="n">
+        <v>16</v>
+      </c>
+      <c r="X65" s="5" t="n">
+        <v>16</v>
+      </c>
+      <c r="Y65" s="5" t="n">
+        <v>56</v>
+      </c>
+      <c r="Z65" s="5" t="n">
+        <v>24</v>
+      </c>
+      <c r="AA65" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB65" s="5" t="n">
+        <v>17</v>
+      </c>
+      <c r="AC65" s="5" t="n">
+        <v>19</v>
+      </c>
+      <c r="AD65" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="AE65" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="66">
+      <c r="A66" s="25"/>
+      <c r="B66" s="8"/>
+      <c r="C66" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D66" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E66" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F66" s="13"/>
+      <c r="G66" s="13"/>
+      <c r="H66" s="13"/>
+      <c r="I66" s="13"/>
+      <c r="J66" s="13" t="n">
+        <v>5</v>
+      </c>
+      <c r="K66" s="13" t="n">
+        <v>6</v>
+      </c>
+      <c r="L66" s="13" t="n">
+        <v>7</v>
+      </c>
+      <c r="M66" s="13" t="n">
+        <v>8</v>
+      </c>
+      <c r="N66" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="O66" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="P66" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q66" s="11"/>
+      <c r="R66" s="11"/>
+      <c r="S66" s="11"/>
+      <c r="T66" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="U66" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="V66" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="W66" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="X66" s="7"/>
+      <c r="Y66" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z66" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA66" s="7"/>
+      <c r="AB66" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="AC66" s="7"/>
+      <c r="AD66" s="7"/>
+      <c r="AE66" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF66" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="17.6" outlineLevel="0" r="68">
+      <c r="A68" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B68" s="5" t="n">
+        <v>14</v>
+      </c>
+      <c r="C68" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="D68" s="5" t="n">
+        <v>28</v>
+      </c>
+      <c r="E68" s="5" t="n">
+        <v>24</v>
+      </c>
+      <c r="F68" s="5" t="n">
+        <v>38</v>
+      </c>
+      <c r="G68" s="5" t="n">
+        <v>43</v>
+      </c>
+      <c r="H68" s="5" t="n">
+        <v>13</v>
+      </c>
+      <c r="I68" s="5" t="n">
+        <v>39</v>
+      </c>
+      <c r="J68" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="K68" s="5" t="n">
+        <v>59</v>
+      </c>
+      <c r="L68" s="5" t="n">
+        <v>46</v>
+      </c>
+      <c r="M68" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="N68" s="5" t="n">
+        <v>13</v>
+      </c>
+      <c r="O68" s="5" t="n">
+        <v>18</v>
+      </c>
+      <c r="P68" s="5" t="n">
+        <v>43</v>
+      </c>
+      <c r="S68" s="27"/>
+      <c r="T68" s="27"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="69">
+      <c r="A69" s="25"/>
+      <c r="B69" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C69" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D69" s="10"/>
+      <c r="E69" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="F69" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="G69" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="H69" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="I69" s="9"/>
+      <c r="J69" s="9"/>
+      <c r="K69" s="9"/>
+      <c r="L69" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="M69" s="7"/>
+      <c r="N69" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="O69" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="P69" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q69" s="7"/>
+      <c r="R69" s="7"/>
+      <c r="S69" s="7"/>
+      <c r="T69" s="7"/>
+      <c r="U69" s="7"/>
+      <c r="V69" s="7"/>
+      <c r="W69" s="7"/>
+      <c r="X69" s="7"/>
+      <c r="Y69" s="7"/>
+      <c r="Z69" s="7"/>
+      <c r="AA69" s="7"/>
+      <c r="AB69" s="7"/>
+      <c r="AC69" s="7"/>
+      <c r="AD69" s="10"/>
+      <c r="AE69" s="10"/>
+      <c r="AF69" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="O24:P24"/>
-    <mergeCell ref="R24:S24"/>
+    <mergeCell ref="O39:P39"/>
+    <mergeCell ref="R39:S39"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
@@ -7165,40 +7536,40 @@
   <dimension ref="A1:AF74"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A52" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <selection activeCell="N78" activeCellId="0" pane="topLeft" sqref="N78"/>
+      <selection activeCell="N78" activeCellId="1" pane="topLeft" sqref="AE3:AF3 N78"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.5254901960784"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="5.16470588235294"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="4.85490196078431"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="5.6078431372549"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="5.31764705882353"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="5" width="4.54901960784314"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="4.38823529411765"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="5" width="4.85490196078431"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="5" width="5.16470588235294"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="5" width="5.6078431372549"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="5" width="4.69411764705882"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="5" width="5.6078431372549"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="5" width="5.01176470588235"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="5" width="4.85490196078431"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="5" width="5.16470588235294"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="5" width="4.69411764705882"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="5" width="4.85490196078431"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="5" width="5.90588235294118"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="5" width="5.6078431372549"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="5" width="4.85490196078431"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="5" width="4.69411764705882"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="5" width="5.45490196078431"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="5" width="5.31764705882353"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="5" width="5.16470588235294"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="5" width="4.38823529411765"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="5" width="4.69411764705882"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="5" width="5.31764705882353"/>
-    <col collapsed="false" hidden="false" max="31" min="30" style="5" width="5.16470588235294"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="5" width="5.75294117647059"/>
-    <col collapsed="false" hidden="false" max="257" min="33" style="0" width="8.68235294117647"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.6039215686275"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="5.1921568627451"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="4.88235294117647"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="5.63529411764706"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="5.34509803921569"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="5" width="4.57647058823529"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="4.41176470588235"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="5" width="4.88235294117647"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="5" width="5.1921568627451"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="5" width="5.63529411764706"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="5" width="4.72156862745098"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="5" width="5.63529411764706"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="5" width="5.03921568627451"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="5" width="4.88235294117647"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="5" width="5.1921568627451"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="5" width="4.72156862745098"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="5" width="4.88235294117647"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="5" width="5.94117647058824"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="5" width="5.63529411764706"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="5" width="4.88235294117647"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="5" width="4.72156862745098"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="5" width="5.48235294117647"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="5" width="5.34509803921569"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="5" width="5.1921568627451"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="5" width="4.41176470588235"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="5" width="4.72156862745098"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="5" width="5.34509803921569"/>
+    <col collapsed="false" hidden="false" max="31" min="30" style="5" width="5.1921568627451"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="5" width="5.78039215686275"/>
+    <col collapsed="false" hidden="false" max="257" min="33" style="0" width="8.72941176470588"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
@@ -7338,12 +7709,12 @@
       <c r="V3" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="W3" s="31" t="s">
+      <c r="W3" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="X3" s="31"/>
-      <c r="Y3" s="31"/>
-      <c r="Z3" s="31"/>
+      <c r="X3" s="32"/>
+      <c r="Y3" s="32"/>
+      <c r="Z3" s="32"/>
       <c r="AA3" s="20" t="s">
         <v>49</v>
       </c>
@@ -9116,7 +9487,7 @@
       <c r="S73" s="27"/>
       <c r="T73" s="27"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.25" outlineLevel="0" r="74">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="74">
       <c r="A74" s="25"/>
       <c r="B74" s="7" t="n">
         <v>1</v>
@@ -9189,41 +9560,41 @@
   <dimension ref="A1:AF71"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A49" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <selection activeCell="P72" activeCellId="0" pane="topLeft" sqref="P72"/>
+      <selection activeCell="P72" activeCellId="1" pane="topLeft" sqref="AE3:AF3 P72"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.5254901960784"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="5.16470588235294"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="4.69411764705882"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="4.22352941176471"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="4.85490196078431"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="5" width="5.45490196078431"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="4.38823529411765"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="5" width="4.85490196078431"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="5" width="5.01176470588235"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="5" width="5.16470588235294"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="5" width="4.69411764705882"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="5" width="5.31764705882353"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="5" width="5.6078431372549"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="5" width="5.16470588235294"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="5" width="4.85490196078431"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="5" width="5.16470588235294"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="5" width="4.69411764705882"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="5" width="4.85490196078431"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="5" width="5.01176470588235"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="5" width="4.69411764705882"/>
-    <col collapsed="false" hidden="false" max="23" min="22" style="5" width="5.31764705882353"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="5" width="5.45490196078431"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="5" width="4.69411764705882"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="5" width="4.85490196078431"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="5" width="5.31764705882353"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="5" width="4.85490196078431"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="5" width="4.08627450980392"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="5" width="3.92549019607843"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="5" width="5.01176470588235"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="5" width="5.6078431372549"/>
-    <col collapsed="false" hidden="false" max="257" min="33" style="0" width="8.68235294117647"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.6039215686275"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="5.1921568627451"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="4.72156862745098"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="4.24313725490196"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="4.88235294117647"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="5" width="5.48235294117647"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="4.41176470588235"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="5" width="4.88235294117647"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="5" width="5.03921568627451"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="5" width="5.1921568627451"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="5" width="4.72156862745098"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="5" width="5.34509803921569"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="5" width="5.63529411764706"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="5" width="5.1921568627451"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="5" width="4.88235294117647"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="5" width="5.1921568627451"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="5" width="4.72156862745098"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="5" width="4.88235294117647"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="5" width="5.03921568627451"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="5" width="4.72156862745098"/>
+    <col collapsed="false" hidden="false" max="23" min="22" style="5" width="5.34509803921569"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="5" width="5.48235294117647"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="5" width="4.72156862745098"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="5" width="4.88235294117647"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="5" width="5.34509803921569"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="5" width="4.88235294117647"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="5" width="4.10588235294118"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="5" width="3.94509803921569"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="5" width="5.03921568627451"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="5" width="5.63529411764706"/>
+    <col collapsed="false" hidden="false" max="257" min="33" style="0" width="8.72941176470588"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
@@ -11069,7 +11440,7 @@
       <c r="S70" s="27"/>
       <c r="T70" s="27"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.25" outlineLevel="0" r="71">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="71">
       <c r="A71" s="25"/>
       <c r="B71" s="11"/>
       <c r="C71" s="13" t="n">
@@ -11145,39 +11516,39 @@
   <dimension ref="A1:AF28"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A7" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <selection activeCell="P28" activeCellId="0" pane="topLeft" sqref="P28"/>
+      <selection activeCell="P28" activeCellId="1" pane="topLeft" sqref="AE3:AF3 P28"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.5254901960784"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="5.45490196078431"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="5.16470588235294"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="5.31764705882353"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="4.85490196078431"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="5" width="5.45490196078431"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="4.38823529411765"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="5" width="4.85490196078431"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="5" width="5.31764705882353"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="5" width="5.16470588235294"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="5" width="4.69411764705882"/>
-    <col collapsed="false" hidden="false" max="14" min="13" style="5" width="5.6078431372549"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="5" width="5.01176470588235"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="5" width="5.16470588235294"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="5" width="4.38823529411765"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="5" width="5.45490196078431"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="5" width="4.85490196078431"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="5" width="5.45490196078431"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="5" width="5.6078431372549"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="5" width="5.01176470588235"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="5" width="5.6078431372549"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="5" width="4.69411764705882"/>
-    <col collapsed="false" hidden="false" max="26" min="25" style="5" width="4.54901960784314"/>
-    <col collapsed="false" hidden="false" max="28" min="27" style="5" width="4.38823529411765"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="5" width="5.01176470588235"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="5" width="5.16470588235294"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="5" width="4.85490196078431"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="5" width="5.31764705882353"/>
-    <col collapsed="false" hidden="false" max="257" min="33" style="0" width="8.68235294117647"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.6039215686275"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="5.48235294117647"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="5.1921568627451"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="5.34509803921569"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="4.88235294117647"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="5" width="5.48235294117647"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="4.41176470588235"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="5" width="4.88235294117647"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="5" width="5.34509803921569"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="5" width="5.1921568627451"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="5" width="4.72156862745098"/>
+    <col collapsed="false" hidden="false" max="14" min="13" style="5" width="5.63529411764706"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="5" width="5.03921568627451"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="5" width="5.1921568627451"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="5" width="4.41176470588235"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="5" width="5.48235294117647"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="5" width="4.88235294117647"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="5" width="5.48235294117647"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="5" width="5.63529411764706"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="5" width="5.03921568627451"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="5" width="5.63529411764706"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="5" width="4.72156862745098"/>
+    <col collapsed="false" hidden="false" max="26" min="25" style="5" width="4.57647058823529"/>
+    <col collapsed="false" hidden="false" max="28" min="27" style="5" width="4.41176470588235"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="5" width="5.03921568627451"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="5" width="5.1921568627451"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="5" width="4.88235294117647"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="5" width="5.34509803921569"/>
+    <col collapsed="false" hidden="false" max="257" min="33" style="0" width="8.72941176470588"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
@@ -12068,7 +12439,7 @@
       <c r="S27" s="27"/>
       <c r="T27" s="27"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.25" outlineLevel="0" r="28">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="28">
       <c r="A28" s="25"/>
       <c r="B28" s="7" t="n">
         <v>2</v>
@@ -12135,42 +12506,42 @@
   <dimension ref="A1:AF39"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A19" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <selection activeCell="K42" activeCellId="0" pane="topLeft" sqref="K42"/>
+      <selection activeCell="K42" activeCellId="1" pane="topLeft" sqref="AE3:AF3 K42"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.5254901960784"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="4.38823529411765"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="4.85490196078431"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="5.16470588235294"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="4.85490196078431"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="5" width="5.45490196078431"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="4.38823529411765"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="5" width="5.45490196078431"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="5" width="5.90588235294118"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="5" width="5.6078431372549"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="5" width="5.16470588235294"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="5" width="4.69411764705882"/>
-    <col collapsed="false" hidden="false" max="14" min="13" style="5" width="5.6078431372549"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="5" width="4.54901960784314"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="5" width="5.01176470588235"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="5" width="5.6078431372549"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="5" width="6.05882352941176"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="5" width="4.85490196078431"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="5" width="5.90588235294118"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="5" width="5.6078431372549"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="5" width="5.75294117647059"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="5" width="6.21176470588235"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="5" width="5.6078431372549"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="5" width="5.16470588235294"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="5" width="4.85490196078431"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="5" width="4.38823529411765"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="5" width="5.01176470588235"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="5" width="4.08627450980392"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="5" width="4.85490196078431"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="5" width="5.6078431372549"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="5.75294117647059"/>
-    <col collapsed="false" hidden="false" max="257" min="33" style="0" width="8.68235294117647"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.6039215686275"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="4.41176470588235"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="4.88235294117647"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="5.1921568627451"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="4.88235294117647"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="5" width="5.48235294117647"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="4.41176470588235"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="5" width="5.48235294117647"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="5" width="5.94117647058824"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="5" width="5.63529411764706"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="5" width="5.1921568627451"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="5" width="4.72156862745098"/>
+    <col collapsed="false" hidden="false" max="14" min="13" style="5" width="5.63529411764706"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="5" width="4.57647058823529"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="5" width="5.03921568627451"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="5" width="5.63529411764706"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="5" width="6.09411764705882"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="5" width="4.88235294117647"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="5" width="5.94117647058824"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="5" width="5.63529411764706"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="5" width="5.78039215686275"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="5" width="6.25098039215686"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="5" width="5.63529411764706"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="5" width="5.1921568627451"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="5" width="4.88235294117647"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="5" width="4.41176470588235"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="5" width="5.03921568627451"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="5" width="4.10588235294118"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="5" width="4.88235294117647"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="5" width="5.63529411764706"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="5.78039215686275"/>
+    <col collapsed="false" hidden="false" max="257" min="33" style="0" width="8.72941176470588"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
@@ -12441,7 +12812,7 @@
         <v>17</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="12" s="32">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="12" s="33">
       <c r="A12" s="6"/>
       <c r="B12" s="11" t="n">
         <v>7</v>
@@ -12662,7 +13033,7 @@
       <c r="AE15" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="AF15" s="33"/>
+      <c r="AF15" s="34"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="17.6" outlineLevel="0" r="17">
       <c r="A17" s="2" t="s">
@@ -12826,7 +13197,7 @@
         <v>1</v>
       </c>
       <c r="AE18" s="8"/>
-      <c r="AF18" s="34"/>
+      <c r="AF18" s="35"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="17.6" outlineLevel="0" r="20">
       <c r="A20" s="2" t="s">
@@ -12903,7 +13274,7 @@
         <v>1</v>
       </c>
       <c r="AE21" s="7"/>
-      <c r="AF21" s="33"/>
+      <c r="AF21" s="34"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="17.6" outlineLevel="0" r="23">
       <c r="A23" s="2" t="s">
@@ -13057,7 +13428,7 @@
       <c r="AE27" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="AF27" s="35" t="s">
+      <c r="AF27" s="36" t="s">
         <v>32</v>
       </c>
     </row>
@@ -13098,7 +13469,7 @@
       <c r="N29" s="5" t="n">
         <v>29</v>
       </c>
-      <c r="AF29" s="36"/>
+      <c r="AF29" s="37"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="30">
       <c r="A30" s="25"/>
@@ -13170,7 +13541,7 @@
       <c r="AE30" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="AF30" s="33"/>
+      <c r="AF30" s="34"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="17.6" outlineLevel="0" r="32">
       <c r="A32" s="2" t="s">
@@ -13514,7 +13885,7 @@
       <c r="AE36" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="AF36" s="33"/>
+      <c r="AF36" s="34"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="17.6" outlineLevel="0" r="38">
       <c r="A38" s="2" t="s">
@@ -13569,7 +13940,7 @@
       <c r="T38" s="27"/>
       <c r="AF38" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.25" outlineLevel="0" r="39">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="39">
       <c r="A39" s="25"/>
       <c r="B39" s="7" t="n">
         <v>1</v>
@@ -13640,36 +14011,36 @@
   <dimension ref="A1:AF48"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A31" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <selection activeCell="P48" activeCellId="0" pane="topLeft" sqref="P48"/>
+      <selection activeCell="P48" activeCellId="1" pane="topLeft" sqref="AE3:AF3 P48"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.5254901960784"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="5.01176470588235"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="4.08627450980392"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="4.22352941176471"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="4.85490196078431"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="5" width="4.69411764705882"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="5" width="4.38823529411765"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="5" width="4.85490196078431"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="5" width="5.16470588235294"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="5" width="4.69411764705882"/>
-    <col collapsed="false" hidden="false" max="14" min="13" style="5" width="5.6078431372549"/>
-    <col collapsed="false" hidden="false" max="17" min="15" style="5" width="5.01176470588235"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="5" width="4.69411764705882"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="5" width="4.85490196078431"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="5" width="5.90588235294118"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="5" width="5.45490196078431"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="5" width="5.01176470588235"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="5" width="5.16470588235294"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="5" width="4.69411764705882"/>
-    <col collapsed="false" hidden="false" max="26" min="25" style="5" width="4.85490196078431"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="5" width="4.38823529411765"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="5" width="4.54901960784314"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="5" width="5.01176470588235"/>
-    <col collapsed="false" hidden="false" max="31" min="30" style="5" width="4.69411764705882"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="5" width="5.31764705882353"/>
-    <col collapsed="false" hidden="false" max="257" min="33" style="0" width="8.68235294117647"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.6039215686275"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="5.03921568627451"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="4.10588235294118"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="4.24313725490196"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="4.88235294117647"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="5" width="4.72156862745098"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="5" width="4.41176470588235"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="5" width="4.88235294117647"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="5" width="5.1921568627451"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="5" width="4.72156862745098"/>
+    <col collapsed="false" hidden="false" max="14" min="13" style="5" width="5.63529411764706"/>
+    <col collapsed="false" hidden="false" max="17" min="15" style="5" width="5.03921568627451"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="5" width="4.72156862745098"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="5" width="4.88235294117647"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="5" width="5.94117647058824"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="5" width="5.48235294117647"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="5" width="5.03921568627451"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="5" width="5.1921568627451"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="5" width="4.72156862745098"/>
+    <col collapsed="false" hidden="false" max="26" min="25" style="5" width="4.88235294117647"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="5" width="4.41176470588235"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="5" width="4.57647058823529"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="5" width="5.03921568627451"/>
+    <col collapsed="false" hidden="false" max="31" min="30" style="5" width="4.72156862745098"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="5" width="5.34509803921569"/>
+    <col collapsed="false" hidden="false" max="257" min="33" style="0" width="8.72941176470588"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
@@ -14064,14 +14435,14 @@
       <c r="M17" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="N17" s="37" t="s">
+      <c r="N17" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="O17" s="37"/>
-      <c r="P17" s="37"/>
-      <c r="Q17" s="37"/>
-      <c r="R17" s="37"/>
-      <c r="S17" s="37"/>
+      <c r="O17" s="38"/>
+      <c r="P17" s="38"/>
+      <c r="Q17" s="38"/>
+      <c r="R17" s="38"/>
+      <c r="S17" s="38"/>
       <c r="T17" s="7" t="n">
         <v>1</v>
       </c>
@@ -14948,7 +15319,7 @@
       <c r="S47" s="27"/>
       <c r="T47" s="27"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.25" outlineLevel="0" r="48">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="48">
       <c r="A48" s="25"/>
       <c r="B48" s="11"/>
       <c r="C48" s="13"/>
@@ -15018,37 +15389,37 @@
   <dimension ref="A1:AF69"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A40" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <selection activeCell="Q71" activeCellId="0" pane="topLeft" sqref="Q71"/>
+      <selection activeCell="Q71" activeCellId="1" pane="topLeft" sqref="AE3:AF3 Q71"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.5254901960784"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="4.54901960784314"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="5.45490196078431"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="4.22352941176471"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="5" width="4.85490196078431"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="4.38823529411765"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="5" width="5.01176470588235"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="5" width="4.85490196078431"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="5" width="5.16470588235294"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="5" width="4.69411764705882"/>
-    <col collapsed="false" hidden="false" max="14" min="13" style="5" width="5.6078431372549"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="5" width="5.01176470588235"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="5" width="4.85490196078431"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="5" width="5.31764705882353"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="5" width="4.69411764705882"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="5" width="4.85490196078431"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="5" width="5.90588235294118"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="5" width="5.6078431372549"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="5" width="5.01176470588235"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="5" width="5.16470588235294"/>
-    <col collapsed="false" hidden="false" max="25" min="24" style="5" width="4.85490196078431"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="5" width="5.45490196078431"/>
-    <col collapsed="false" hidden="false" max="28" min="27" style="5" width="5.16470588235294"/>
-    <col collapsed="false" hidden="false" max="30" min="29" style="5" width="4.69411764705882"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="5" width="4.38823529411765"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="5" width="5.01176470588235"/>
-    <col collapsed="false" hidden="false" max="257" min="33" style="0" width="8.68235294117647"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.6039215686275"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="4.57647058823529"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="5.48235294117647"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="4.24313725490196"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="5" width="4.88235294117647"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="4.41176470588235"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="5" width="5.03921568627451"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="5" width="4.88235294117647"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="5" width="5.1921568627451"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="5" width="4.72156862745098"/>
+    <col collapsed="false" hidden="false" max="14" min="13" style="5" width="5.63529411764706"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="5" width="5.03921568627451"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="5" width="4.88235294117647"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="5" width="5.34509803921569"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="5" width="4.72156862745098"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="5" width="4.88235294117647"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="5" width="5.94117647058824"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="5" width="5.63529411764706"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="5" width="5.03921568627451"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="5" width="5.1921568627451"/>
+    <col collapsed="false" hidden="false" max="25" min="24" style="5" width="4.88235294117647"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="5" width="5.48235294117647"/>
+    <col collapsed="false" hidden="false" max="28" min="27" style="5" width="5.1921568627451"/>
+    <col collapsed="false" hidden="false" max="30" min="29" style="5" width="4.72156862745098"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="5" width="4.41176470588235"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="5" width="5.03921568627451"/>
+    <col collapsed="false" hidden="false" max="257" min="33" style="0" width="8.72941176470588"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
@@ -15198,12 +15569,12 @@
         <v>1</v>
       </c>
       <c r="V3" s="7"/>
-      <c r="W3" s="31" t="s">
+      <c r="W3" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="X3" s="31"/>
-      <c r="Y3" s="31"/>
-      <c r="Z3" s="31"/>
+      <c r="X3" s="32"/>
+      <c r="Y3" s="32"/>
+      <c r="Z3" s="32"/>
       <c r="AA3" s="20" t="s">
         <v>49</v>
       </c>
@@ -15214,7 +15585,7 @@
       <c r="AF3" s="20"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="17.6" outlineLevel="0" r="4">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="39" t="s">
         <v>16</v>
       </c>
     </row>
@@ -15283,7 +15654,7 @@
       <c r="AF5" s="19"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="17.6" outlineLevel="0" r="7">
-      <c r="A7" s="38" t="s">
+      <c r="A7" s="39" t="s">
         <v>17</v>
       </c>
     </row>
@@ -15344,7 +15715,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="17.6" outlineLevel="0" r="10">
-      <c r="A10" s="38" t="s">
+      <c r="A10" s="39" t="s">
         <v>18</v>
       </c>
     </row>
@@ -15417,7 +15788,7 @@
       <c r="AF11" s="19"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="17.6" outlineLevel="0" r="13">
-      <c r="A13" s="38" t="s">
+      <c r="A13" s="39" t="s">
         <v>19</v>
       </c>
     </row>
@@ -15494,7 +15865,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="17.6" outlineLevel="0" r="16">
-      <c r="A16" s="38" t="s">
+      <c r="A16" s="39" t="s">
         <v>20</v>
       </c>
     </row>
@@ -15559,7 +15930,7 @@
       <c r="AF17" s="19"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="17.6" outlineLevel="0" r="19">
-      <c r="A19" s="38" t="s">
+      <c r="A19" s="39" t="s">
         <v>55</v>
       </c>
     </row>
@@ -16063,14 +16434,14 @@
       <c r="M40" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="N40" s="37" t="s">
+      <c r="N40" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="O40" s="37"/>
-      <c r="P40" s="37"/>
-      <c r="Q40" s="37"/>
-      <c r="R40" s="37"/>
-      <c r="S40" s="37"/>
+      <c r="O40" s="38"/>
+      <c r="P40" s="38"/>
+      <c r="Q40" s="38"/>
+      <c r="R40" s="38"/>
+      <c r="S40" s="38"/>
       <c r="T40" s="7" t="n">
         <v>1</v>
       </c>
@@ -16941,7 +17312,7 @@
       <c r="S68" s="27"/>
       <c r="T68" s="27"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.25" outlineLevel="0" r="69">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="69">
       <c r="A69" s="25"/>
       <c r="B69" s="7" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
update data to 9/2016
</commit_message>
<xml_diff>
--- a/MakeMoney/Thong_Ke/xls/Cau_T2.xlsx
+++ b/MakeMoney/Thong_Ke/xls/Cau_T2.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="66">
   <si>
     <t>Cau so 10</t>
   </si>
@@ -505,7 +505,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
@@ -649,21 +649,6 @@
     <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -694,12 +679,6 @@
     <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -721,6 +700,33 @@
     <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -739,10 +745,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3398,17 +3401,17 @@
       <c r="N36" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="O36" s="49" t="s">
+      <c r="O36" s="68" t="s">
         <v>30</v>
       </c>
-      <c r="P36" s="49"/>
+      <c r="P36" s="68"/>
       <c r="Q36" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="R36" s="49" t="s">
+      <c r="R36" s="68" t="s">
         <v>30</v>
       </c>
-      <c r="S36" s="49"/>
+      <c r="S36" s="68"/>
       <c r="T36" s="23"/>
       <c r="U36" s="23"/>
       <c r="V36" s="23"/>
@@ -5529,17 +5532,17 @@
       <c r="N39" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="O39" s="49" t="s">
+      <c r="O39" s="68" t="s">
         <v>30</v>
       </c>
-      <c r="P39" s="49"/>
+      <c r="P39" s="68"/>
       <c r="Q39" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="R39" s="49" t="s">
+      <c r="R39" s="68" t="s">
         <v>30</v>
       </c>
-      <c r="S39" s="49"/>
+      <c r="S39" s="68"/>
       <c r="T39" s="7">
         <v>1</v>
       </c>
@@ -7642,17 +7645,17 @@
       <c r="N39" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="O39" s="50" t="s">
+      <c r="O39" s="69" t="s">
         <v>30</v>
       </c>
-      <c r="P39" s="50"/>
+      <c r="P39" s="69"/>
       <c r="Q39" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="R39" s="50" t="s">
+      <c r="R39" s="69" t="s">
         <v>30</v>
       </c>
-      <c r="S39" s="50"/>
+      <c r="S39" s="69"/>
       <c r="T39" s="10"/>
       <c r="U39" s="10"/>
       <c r="V39" s="10">
@@ -8953,20 +8956,20 @@
       <c r="V3" s="13">
         <v>5</v>
       </c>
-      <c r="W3" s="51" t="s">
+      <c r="W3" s="70" t="s">
         <v>55</v>
       </c>
-      <c r="X3" s="51"/>
-      <c r="Y3" s="51"/>
-      <c r="Z3" s="51"/>
-      <c r="AA3" s="49" t="s">
+      <c r="X3" s="70"/>
+      <c r="Y3" s="70"/>
+      <c r="Z3" s="70"/>
+      <c r="AA3" s="68" t="s">
         <v>56</v>
       </c>
-      <c r="AB3" s="49"/>
-      <c r="AC3" s="49"/>
-      <c r="AD3" s="49"/>
-      <c r="AE3" s="49"/>
-      <c r="AF3" s="49"/>
+      <c r="AB3" s="68"/>
+      <c r="AC3" s="68"/>
+      <c r="AD3" s="68"/>
+      <c r="AE3" s="68"/>
+      <c r="AF3" s="68"/>
     </row>
     <row r="5" spans="1:32" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -9799,17 +9802,17 @@
       <c r="N42" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="O42" s="49" t="s">
+      <c r="O42" s="68" t="s">
         <v>30</v>
       </c>
-      <c r="P42" s="49"/>
+      <c r="P42" s="68"/>
       <c r="Q42" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="R42" s="49" t="s">
+      <c r="R42" s="68" t="s">
         <v>30</v>
       </c>
-      <c r="S42" s="49"/>
+      <c r="S42" s="68"/>
       <c r="T42" s="7">
         <v>1</v>
       </c>
@@ -11150,14 +11153,14 @@
       <c r="T3" s="8"/>
       <c r="U3" s="8"/>
       <c r="V3" s="8"/>
-      <c r="AA3" s="49" t="s">
+      <c r="AA3" s="68" t="s">
         <v>56</v>
       </c>
-      <c r="AB3" s="49"/>
-      <c r="AC3" s="49"/>
-      <c r="AD3" s="49"/>
-      <c r="AE3" s="49"/>
-      <c r="AF3" s="49"/>
+      <c r="AB3" s="68"/>
+      <c r="AC3" s="68"/>
+      <c r="AD3" s="68"/>
+      <c r="AE3" s="68"/>
+      <c r="AF3" s="68"/>
     </row>
     <row r="4" spans="1:32" ht="18" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -11979,17 +11982,17 @@
       <c r="N41" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="O41" s="49" t="s">
+      <c r="O41" s="68" t="s">
         <v>30</v>
       </c>
-      <c r="P41" s="49"/>
+      <c r="P41" s="68"/>
       <c r="Q41" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="R41" s="49" t="s">
+      <c r="R41" s="68" t="s">
         <v>30</v>
       </c>
-      <c r="S41" s="49"/>
+      <c r="S41" s="68"/>
       <c r="T41" s="8"/>
       <c r="U41" s="8"/>
       <c r="V41" s="8"/>
@@ -14543,17 +14546,17 @@
       <c r="N9" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="O9" s="49" t="s">
+      <c r="O9" s="68" t="s">
         <v>30</v>
       </c>
-      <c r="P9" s="49"/>
+      <c r="P9" s="68"/>
       <c r="Q9" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="R9" s="49" t="s">
+      <c r="R9" s="68" t="s">
         <v>30</v>
       </c>
-      <c r="S9" s="49"/>
+      <c r="S9" s="68"/>
       <c r="T9" s="7">
         <v>1</v>
       </c>
@@ -16363,14 +16366,14 @@
       <c r="M17" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="N17" s="52" t="s">
+      <c r="N17" s="71" t="s">
         <v>56</v>
       </c>
-      <c r="O17" s="52"/>
-      <c r="P17" s="52"/>
-      <c r="Q17" s="52"/>
-      <c r="R17" s="52"/>
-      <c r="S17" s="52"/>
+      <c r="O17" s="71"/>
+      <c r="P17" s="71"/>
+      <c r="Q17" s="71"/>
+      <c r="R17" s="71"/>
+      <c r="S17" s="71"/>
       <c r="T17" s="7">
         <v>1</v>
       </c>
@@ -17487,13 +17490,13 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF150"/>
+  <dimension ref="A1:AF168"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="18" ySplit="14" topLeftCell="U135" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="18" ySplit="14" topLeftCell="U162" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="S1" sqref="S1"/>
       <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
-      <selection pane="bottomRight" activeCell="F140" sqref="F140"/>
+      <selection pane="bottomRight" activeCell="AA171" sqref="AA171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -17629,14 +17632,14 @@
     </row>
     <row r="3" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6"/>
-      <c r="B3" s="49" t="s">
+      <c r="B3" s="68" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="49"/>
-      <c r="G3" s="49"/>
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
+      <c r="F3" s="68"/>
+      <c r="G3" s="68"/>
       <c r="H3" s="7">
         <v>1</v>
       </c>
@@ -17674,20 +17677,20 @@
         <v>1</v>
       </c>
       <c r="V3" s="7"/>
-      <c r="W3" s="51" t="s">
+      <c r="W3" s="70" t="s">
         <v>55</v>
       </c>
-      <c r="X3" s="51"/>
-      <c r="Y3" s="51"/>
-      <c r="Z3" s="51"/>
-      <c r="AA3" s="49" t="s">
+      <c r="X3" s="70"/>
+      <c r="Y3" s="70"/>
+      <c r="Z3" s="70"/>
+      <c r="AA3" s="68" t="s">
         <v>56</v>
       </c>
-      <c r="AB3" s="49"/>
-      <c r="AC3" s="49"/>
-      <c r="AD3" s="49"/>
-      <c r="AE3" s="49"/>
-      <c r="AF3" s="49"/>
+      <c r="AB3" s="68"/>
+      <c r="AC3" s="68"/>
+      <c r="AD3" s="68"/>
+      <c r="AE3" s="68"/>
+      <c r="AF3" s="68"/>
     </row>
     <row r="4" spans="1:32" ht="18" x14ac:dyDescent="0.25">
       <c r="A4" s="34" t="s">
@@ -18541,14 +18544,14 @@
       <c r="M40" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="N40" s="52" t="s">
+      <c r="N40" s="71" t="s">
         <v>56</v>
       </c>
-      <c r="O40" s="52"/>
-      <c r="P40" s="52"/>
-      <c r="Q40" s="52"/>
-      <c r="R40" s="52"/>
-      <c r="S40" s="52"/>
+      <c r="O40" s="71"/>
+      <c r="P40" s="71"/>
+      <c r="Q40" s="71"/>
+      <c r="R40" s="71"/>
+      <c r="S40" s="71"/>
       <c r="T40" s="7">
         <v>1</v>
       </c>
@@ -19717,15 +19720,15 @@
     </row>
     <row r="75" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="6"/>
-      <c r="B75" s="53" t="s">
+      <c r="B75" s="81" t="s">
         <v>60</v>
       </c>
-      <c r="C75" s="53"/>
+      <c r="C75" s="81"/>
       <c r="D75" s="7"/>
-      <c r="E75" s="53" t="s">
+      <c r="E75" s="81" t="s">
         <v>60</v>
       </c>
-      <c r="F75" s="53"/>
+      <c r="F75" s="81"/>
       <c r="G75" s="7"/>
       <c r="H75" s="7"/>
       <c r="I75" s="7"/>
@@ -20194,12 +20197,12 @@
       <c r="M96" s="43"/>
       <c r="N96" s="43"/>
       <c r="O96" s="43"/>
-      <c r="P96" s="54"/>
-      <c r="Q96" s="54"/>
-      <c r="R96" s="54">
+      <c r="P96" s="49"/>
+      <c r="Q96" s="49"/>
+      <c r="R96" s="49">
         <v>6</v>
       </c>
-      <c r="S96" s="54">
+      <c r="S96" s="49">
         <v>7</v>
       </c>
       <c r="T96" s="7">
@@ -20348,12 +20351,12 @@
       <c r="Y102" s="7">
         <v>1</v>
       </c>
-      <c r="Z102" s="57"/>
-      <c r="AA102" s="57">
-        <v>1</v>
-      </c>
-      <c r="AB102" s="57"/>
-      <c r="AC102" s="57"/>
+      <c r="Z102" s="52"/>
+      <c r="AA102" s="52">
+        <v>1</v>
+      </c>
+      <c r="AB102" s="52"/>
+      <c r="AC102" s="52"/>
       <c r="AD102" s="7">
         <v>1</v>
       </c>
@@ -20371,15 +20374,15 @@
       <c r="B105" s="7">
         <v>1</v>
       </c>
-      <c r="C105" s="55"/>
-      <c r="D105" s="55"/>
-      <c r="E105" s="60"/>
-      <c r="F105" s="60"/>
-      <c r="G105" s="56"/>
-      <c r="H105" s="60"/>
-      <c r="I105" s="55"/>
-      <c r="J105" s="61"/>
-      <c r="K105" s="61">
+      <c r="C105" s="50"/>
+      <c r="D105" s="50"/>
+      <c r="E105" s="55"/>
+      <c r="F105" s="55"/>
+      <c r="G105" s="51"/>
+      <c r="H105" s="55"/>
+      <c r="I105" s="50"/>
+      <c r="J105" s="56"/>
+      <c r="K105" s="56">
         <v>9</v>
       </c>
       <c r="L105" s="44">
@@ -20388,14 +20391,14 @@
       <c r="M105" s="43"/>
       <c r="N105" s="43"/>
       <c r="O105" s="43"/>
-      <c r="P105" s="56"/>
-      <c r="Q105" s="56">
+      <c r="P105" s="51"/>
+      <c r="Q105" s="51">
         <v>0</v>
       </c>
-      <c r="R105" s="56">
+      <c r="R105" s="51">
         <v>6</v>
       </c>
-      <c r="S105" s="57">
+      <c r="S105" s="52">
         <v>1</v>
       </c>
       <c r="T105" s="7"/>
@@ -20413,14 +20416,14 @@
       <c r="AB105" s="7">
         <v>1</v>
       </c>
-      <c r="AC105" s="57">
-        <v>1</v>
-      </c>
-      <c r="AD105" s="58">
-        <v>1</v>
-      </c>
-      <c r="AE105" s="58"/>
-      <c r="AF105" s="58"/>
+      <c r="AC105" s="52">
+        <v>1</v>
+      </c>
+      <c r="AD105" s="53">
+        <v>1</v>
+      </c>
+      <c r="AE105" s="53"/>
+      <c r="AF105" s="53"/>
     </row>
     <row r="107" spans="1:32" ht="18" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
@@ -20441,12 +20444,12 @@
       <c r="E108" s="10">
         <v>1</v>
       </c>
-      <c r="F108" s="61"/>
+      <c r="F108" s="56"/>
       <c r="G108" s="45"/>
-      <c r="H108" s="61"/>
-      <c r="I108" s="55"/>
-      <c r="J108" s="55"/>
-      <c r="K108" s="55">
+      <c r="H108" s="56"/>
+      <c r="I108" s="50"/>
+      <c r="J108" s="50"/>
+      <c r="K108" s="50">
         <v>6</v>
       </c>
       <c r="L108" s="7">
@@ -20500,17 +20503,17 @@
     </row>
     <row r="111" spans="1:32" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="6"/>
-      <c r="B111" s="63">
-        <v>1</v>
-      </c>
-      <c r="C111" s="63"/>
+      <c r="B111" s="58">
+        <v>1</v>
+      </c>
+      <c r="C111" s="58"/>
       <c r="D111" s="7">
         <v>1</v>
       </c>
-      <c r="E111" s="63">
-        <v>1</v>
-      </c>
-      <c r="F111" s="63">
+      <c r="E111" s="58">
+        <v>1</v>
+      </c>
+      <c r="F111" s="58">
         <v>1</v>
       </c>
       <c r="G111" s="7"/>
@@ -20526,32 +20529,32 @@
       <c r="M111" s="36">
         <v>1</v>
       </c>
-      <c r="N111" s="62">
-        <v>1</v>
-      </c>
-      <c r="O111" s="62">
-        <v>1</v>
-      </c>
-      <c r="P111" s="62">
-        <v>1</v>
-      </c>
-      <c r="Q111" s="64" t="s">
+      <c r="N111" s="57">
+        <v>1</v>
+      </c>
+      <c r="O111" s="57">
+        <v>1</v>
+      </c>
+      <c r="P111" s="57">
+        <v>1</v>
+      </c>
+      <c r="Q111" s="72" t="s">
         <v>64</v>
       </c>
-      <c r="R111" s="65"/>
-      <c r="S111" s="65"/>
-      <c r="T111" s="65"/>
-      <c r="U111" s="65"/>
-      <c r="V111" s="65"/>
-      <c r="W111" s="66" t="s">
+      <c r="R111" s="73"/>
+      <c r="S111" s="73"/>
+      <c r="T111" s="73"/>
+      <c r="U111" s="73"/>
+      <c r="V111" s="73"/>
+      <c r="W111" s="74" t="s">
         <v>60</v>
       </c>
-      <c r="X111" s="66"/>
-      <c r="Y111" s="66"/>
-      <c r="Z111" s="66"/>
-      <c r="AA111" s="66"/>
-      <c r="AB111" s="66"/>
-      <c r="AC111" s="66"/>
+      <c r="X111" s="74"/>
+      <c r="Y111" s="74"/>
+      <c r="Z111" s="74"/>
+      <c r="AA111" s="74"/>
+      <c r="AB111" s="74"/>
+      <c r="AC111" s="74"/>
     </row>
     <row r="113" spans="1:32" ht="18" x14ac:dyDescent="0.25">
       <c r="A113" s="34" t="s">
@@ -20855,17 +20858,17 @@
       <c r="V126" s="7">
         <v>1</v>
       </c>
-      <c r="W126" s="67"/>
-      <c r="X126" s="67"/>
-      <c r="Y126" s="67"/>
-      <c r="Z126" s="67"/>
+      <c r="W126" s="60"/>
+      <c r="X126" s="60"/>
+      <c r="Y126" s="60"/>
+      <c r="Z126" s="60"/>
       <c r="AA126" s="7">
         <v>1</v>
       </c>
-      <c r="AB126" s="67"/>
-      <c r="AC126" s="67"/>
-      <c r="AD126" s="67"/>
-      <c r="AE126" s="67"/>
+      <c r="AB126" s="60"/>
+      <c r="AC126" s="60"/>
+      <c r="AD126" s="60"/>
+      <c r="AE126" s="60"/>
       <c r="AF126" s="7">
         <v>1</v>
       </c>
@@ -20884,10 +20887,10 @@
       <c r="D129" s="7">
         <v>1</v>
       </c>
-      <c r="E129" s="67"/>
-      <c r="F129" s="68"/>
-      <c r="G129" s="68"/>
-      <c r="H129" s="68"/>
+      <c r="E129" s="60"/>
+      <c r="F129" s="61"/>
+      <c r="G129" s="61"/>
+      <c r="H129" s="61"/>
       <c r="I129" s="7">
         <v>1</v>
       </c>
@@ -20904,19 +20907,19 @@
       <c r="P129" s="45"/>
       <c r="Q129" s="45"/>
       <c r="R129" s="43"/>
-      <c r="S129" s="54"/>
-      <c r="T129" s="54"/>
-      <c r="U129" s="54"/>
-      <c r="V129" s="54">
+      <c r="S129" s="49"/>
+      <c r="T129" s="49"/>
+      <c r="U129" s="49"/>
+      <c r="V129" s="49">
         <v>7</v>
       </c>
       <c r="W129" s="7">
         <v>1</v>
       </c>
-      <c r="X129" s="67"/>
-      <c r="Y129" s="67"/>
-      <c r="Z129" s="67"/>
-      <c r="AA129" s="67"/>
+      <c r="X129" s="60"/>
+      <c r="Y129" s="60"/>
+      <c r="Z129" s="60"/>
+      <c r="AA129" s="60"/>
       <c r="AB129" s="7">
         <v>1</v>
       </c>
@@ -20951,10 +20954,10 @@
       <c r="H132" s="7">
         <v>1</v>
       </c>
-      <c r="I132" s="67"/>
-      <c r="J132" s="67"/>
-      <c r="K132" s="67"/>
-      <c r="L132" s="67"/>
+      <c r="I132" s="60"/>
+      <c r="J132" s="60"/>
+      <c r="K132" s="60"/>
+      <c r="L132" s="60"/>
       <c r="M132" s="7">
         <v>1</v>
       </c>
@@ -21018,10 +21021,10 @@
       <c r="E135" s="10">
         <v>1</v>
       </c>
-      <c r="F135" s="69"/>
-      <c r="G135" s="69"/>
-      <c r="H135" s="69"/>
-      <c r="I135" s="69"/>
+      <c r="F135" s="62"/>
+      <c r="G135" s="62"/>
+      <c r="H135" s="62"/>
+      <c r="I135" s="62"/>
       <c r="J135" s="10">
         <v>1</v>
       </c>
@@ -21120,16 +21123,16 @@
       <c r="Y138" s="7">
         <v>1</v>
       </c>
-      <c r="Z138" s="57">
-        <v>1</v>
-      </c>
-      <c r="AA138" s="57"/>
-      <c r="AB138" s="57">
-        <v>1</v>
-      </c>
-      <c r="AC138" s="80"/>
-      <c r="AD138" s="67"/>
-      <c r="AE138" s="67"/>
+      <c r="Z138" s="52">
+        <v>1</v>
+      </c>
+      <c r="AA138" s="52"/>
+      <c r="AB138" s="52">
+        <v>1</v>
+      </c>
+      <c r="AC138" s="67"/>
+      <c r="AD138" s="60"/>
+      <c r="AE138" s="60"/>
     </row>
     <row r="140" spans="1:32" ht="18" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
@@ -21140,24 +21143,24 @@
     </row>
     <row r="141" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A141" s="24"/>
-      <c r="B141" s="67"/>
+      <c r="B141" s="60"/>
       <c r="C141" s="10">
         <v>1</v>
       </c>
       <c r="D141" s="10"/>
-      <c r="E141" s="58">
-        <v>1</v>
-      </c>
-      <c r="F141" s="58"/>
-      <c r="G141" s="57">
-        <v>1</v>
-      </c>
-      <c r="H141" s="58"/>
+      <c r="E141" s="53">
+        <v>1</v>
+      </c>
+      <c r="F141" s="53"/>
+      <c r="G141" s="52">
+        <v>1</v>
+      </c>
+      <c r="H141" s="53"/>
       <c r="I141" s="10">
         <v>1</v>
       </c>
-      <c r="J141" s="59"/>
-      <c r="K141" s="59"/>
+      <c r="J141" s="54"/>
+      <c r="K141" s="54"/>
       <c r="L141" s="44">
         <v>1</v>
       </c>
@@ -21168,12 +21171,12 @@
       <c r="O141" s="7">
         <v>1</v>
       </c>
-      <c r="P141" s="57"/>
-      <c r="Q141" s="57"/>
-      <c r="R141" s="57">
-        <v>1</v>
-      </c>
-      <c r="S141" s="57">
+      <c r="P141" s="52"/>
+      <c r="Q141" s="52"/>
+      <c r="R141" s="52">
+        <v>1</v>
+      </c>
+      <c r="S141" s="52">
         <v>1</v>
       </c>
       <c r="T141" s="7">
@@ -21193,10 +21196,10 @@
       </c>
       <c r="AA141" s="43"/>
       <c r="AB141" s="43"/>
-      <c r="AC141" s="56"/>
-      <c r="AD141" s="60"/>
-      <c r="AE141" s="60"/>
-      <c r="AF141" s="60"/>
+      <c r="AC141" s="51"/>
+      <c r="AD141" s="55"/>
+      <c r="AE141" s="55"/>
+      <c r="AF141" s="55"/>
     </row>
     <row r="143" spans="1:32" ht="18" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
@@ -21208,21 +21211,21 @@
     <row r="144" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A144" s="24"/>
       <c r="B144" s="43"/>
-      <c r="C144" s="55">
+      <c r="C144" s="50">
         <v>8</v>
       </c>
       <c r="D144" s="10">
         <v>1</v>
       </c>
-      <c r="E144" s="58"/>
-      <c r="F144" s="58"/>
-      <c r="G144" s="57">
-        <v>1</v>
-      </c>
-      <c r="H144" s="70"/>
-      <c r="I144" s="71"/>
-      <c r="J144" s="72"/>
-      <c r="K144" s="72"/>
+      <c r="E144" s="53"/>
+      <c r="F144" s="53"/>
+      <c r="G144" s="52">
+        <v>1</v>
+      </c>
+      <c r="H144" s="63"/>
+      <c r="I144" s="64"/>
+      <c r="J144" s="65"/>
+      <c r="K144" s="65"/>
       <c r="L144" s="44">
         <v>1</v>
       </c>
@@ -21233,16 +21236,16 @@
         <v>1</v>
       </c>
       <c r="O144" s="7"/>
-      <c r="P144" s="57">
-        <v>1</v>
-      </c>
-      <c r="Q144" s="57">
-        <v>1</v>
-      </c>
-      <c r="R144" s="57">
-        <v>1</v>
-      </c>
-      <c r="S144" s="57">
+      <c r="P144" s="52">
+        <v>1</v>
+      </c>
+      <c r="Q144" s="52">
+        <v>1</v>
+      </c>
+      <c r="R144" s="52">
+        <v>1</v>
+      </c>
+      <c r="S144" s="52">
         <v>1</v>
       </c>
       <c r="T144" s="7"/>
@@ -21252,20 +21255,20 @@
       <c r="V144" s="44">
         <v>1</v>
       </c>
-      <c r="W144" s="68"/>
-      <c r="X144" s="67"/>
-      <c r="Y144" s="67"/>
-      <c r="Z144" s="67"/>
+      <c r="W144" s="61"/>
+      <c r="X144" s="60"/>
+      <c r="Y144" s="60"/>
+      <c r="Z144" s="60"/>
       <c r="AA144" s="7">
         <v>1</v>
       </c>
       <c r="AB144" s="7"/>
-      <c r="AC144" s="57"/>
-      <c r="AD144" s="58">
-        <v>1</v>
-      </c>
-      <c r="AE144" s="58"/>
-      <c r="AF144" s="58"/>
+      <c r="AC144" s="52"/>
+      <c r="AD144" s="53">
+        <v>1</v>
+      </c>
+      <c r="AE144" s="53"/>
+      <c r="AF144" s="53"/>
     </row>
     <row r="146" spans="1:32" ht="18" x14ac:dyDescent="0.25">
       <c r="A146" s="34" t="s">
@@ -21284,18 +21287,18 @@
       <c r="G147" s="13">
         <v>5</v>
       </c>
-      <c r="H147" s="73" t="s">
+      <c r="H147" s="75" t="s">
         <v>60</v>
       </c>
-      <c r="I147" s="74"/>
-      <c r="J147" s="74"/>
-      <c r="K147" s="75"/>
-      <c r="L147" s="76"/>
-      <c r="M147" s="77"/>
-      <c r="N147" s="77"/>
-      <c r="O147" s="77"/>
-      <c r="P147" s="77"/>
-      <c r="Q147" s="78"/>
+      <c r="I147" s="76"/>
+      <c r="J147" s="76"/>
+      <c r="K147" s="77"/>
+      <c r="L147" s="78"/>
+      <c r="M147" s="79"/>
+      <c r="N147" s="79"/>
+      <c r="O147" s="79"/>
+      <c r="P147" s="79"/>
+      <c r="Q147" s="80"/>
       <c r="R147" s="7">
         <v>1</v>
       </c>
@@ -21307,10 +21310,10 @@
       <c r="V147" s="7">
         <v>1</v>
       </c>
-      <c r="W147" s="67"/>
-      <c r="X147" s="67"/>
-      <c r="Y147" s="67"/>
-      <c r="Z147" s="79"/>
+      <c r="W147" s="60"/>
+      <c r="X147" s="60"/>
+      <c r="Y147" s="60"/>
+      <c r="Z147" s="66"/>
       <c r="AA147" s="37">
         <v>1</v>
       </c>
@@ -21388,8 +21391,414 @@
       <c r="AD150" s="37">
         <v>1</v>
       </c>
-      <c r="AE150" s="37"/>
-      <c r="AF150" s="37"/>
+      <c r="AE150" s="66"/>
+      <c r="AF150" s="66"/>
+    </row>
+    <row r="152" spans="1:32" ht="18" x14ac:dyDescent="0.25">
+      <c r="A152" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="S152" s="26"/>
+      <c r="U152" s="26"/>
+      <c r="V152" s="26"/>
+    </row>
+    <row r="153" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A153" s="24"/>
+      <c r="B153" s="60"/>
+      <c r="C153" s="60"/>
+      <c r="D153" s="59">
+        <v>1</v>
+      </c>
+      <c r="E153" s="59">
+        <v>1</v>
+      </c>
+      <c r="F153" s="43"/>
+      <c r="G153" s="43"/>
+      <c r="H153" s="43"/>
+      <c r="I153" s="43"/>
+      <c r="J153" s="43">
+        <v>5</v>
+      </c>
+      <c r="K153" s="59">
+        <v>1</v>
+      </c>
+      <c r="L153" s="59">
+        <v>1</v>
+      </c>
+      <c r="M153" s="59">
+        <v>1</v>
+      </c>
+      <c r="N153" s="59"/>
+      <c r="O153" s="59"/>
+      <c r="P153" s="59">
+        <v>1</v>
+      </c>
+      <c r="Q153" s="59"/>
+      <c r="R153" s="44"/>
+      <c r="S153" s="44"/>
+      <c r="T153" s="44"/>
+      <c r="U153" s="59">
+        <v>1</v>
+      </c>
+      <c r="V153" s="59"/>
+      <c r="W153" s="59"/>
+      <c r="X153" s="59">
+        <v>1</v>
+      </c>
+      <c r="Y153" s="59"/>
+      <c r="Z153" s="52">
+        <v>1</v>
+      </c>
+      <c r="AA153" s="51"/>
+      <c r="AB153" s="51"/>
+      <c r="AC153" s="51"/>
+      <c r="AD153" s="43"/>
+      <c r="AE153" s="43">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="155" spans="1:32" ht="18" x14ac:dyDescent="0.25">
+      <c r="A155" s="34" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="156" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A156" s="6"/>
+      <c r="B156" s="59">
+        <v>1</v>
+      </c>
+      <c r="C156" s="59"/>
+      <c r="D156" s="59">
+        <v>1</v>
+      </c>
+      <c r="E156" s="59"/>
+      <c r="F156" s="59">
+        <v>1</v>
+      </c>
+      <c r="G156" s="43"/>
+      <c r="H156" s="43"/>
+      <c r="I156" s="43"/>
+      <c r="J156" s="45"/>
+      <c r="K156" s="45"/>
+      <c r="L156" s="45"/>
+      <c r="M156" s="43">
+        <v>7</v>
+      </c>
+      <c r="N156" s="44">
+        <v>1</v>
+      </c>
+      <c r="O156" s="61"/>
+      <c r="P156" s="61"/>
+      <c r="Q156" s="60"/>
+      <c r="R156" s="60"/>
+      <c r="S156" s="43"/>
+      <c r="T156" s="45">
+        <v>6</v>
+      </c>
+      <c r="U156" s="44">
+        <v>1</v>
+      </c>
+      <c r="V156" s="44">
+        <v>1</v>
+      </c>
+      <c r="W156" s="59">
+        <v>1</v>
+      </c>
+      <c r="X156" s="44">
+        <v>1</v>
+      </c>
+      <c r="Y156" s="44">
+        <v>1</v>
+      </c>
+      <c r="Z156" s="45"/>
+      <c r="AA156" s="43"/>
+      <c r="AB156" s="13"/>
+      <c r="AC156" s="13"/>
+      <c r="AD156" s="13">
+        <v>5</v>
+      </c>
+      <c r="AE156" s="37">
+        <v>1</v>
+      </c>
+      <c r="AF156" s="37"/>
+    </row>
+    <row r="158" spans="1:32" ht="18" x14ac:dyDescent="0.25">
+      <c r="A158" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="S158" s="26"/>
+      <c r="U158" s="26"/>
+      <c r="V158" s="26"/>
+    </row>
+    <row r="159" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A159" s="24"/>
+      <c r="B159" s="59"/>
+      <c r="C159" s="59">
+        <v>1</v>
+      </c>
+      <c r="D159" s="59"/>
+      <c r="E159" s="59">
+        <v>0</v>
+      </c>
+      <c r="F159" s="59">
+        <v>0</v>
+      </c>
+      <c r="G159" s="59"/>
+      <c r="H159" s="59"/>
+      <c r="I159" s="59">
+        <v>1</v>
+      </c>
+      <c r="J159" s="59"/>
+      <c r="K159" s="59">
+        <v>1</v>
+      </c>
+      <c r="L159" s="59">
+        <v>1</v>
+      </c>
+      <c r="M159" s="59">
+        <v>1</v>
+      </c>
+      <c r="N159" s="59"/>
+      <c r="O159" s="59"/>
+      <c r="P159" s="59">
+        <v>1</v>
+      </c>
+      <c r="Q159" s="59"/>
+      <c r="R159" s="44"/>
+      <c r="S159" s="44">
+        <v>1</v>
+      </c>
+      <c r="T159" s="44">
+        <v>1</v>
+      </c>
+      <c r="U159" s="59"/>
+      <c r="V159" s="59">
+        <v>1</v>
+      </c>
+      <c r="W159" s="59"/>
+      <c r="X159" s="59">
+        <v>1</v>
+      </c>
+      <c r="Y159" s="59"/>
+      <c r="Z159" s="52"/>
+      <c r="AA159" s="52">
+        <v>1</v>
+      </c>
+      <c r="AB159" s="52"/>
+      <c r="AC159" s="52">
+        <v>1</v>
+      </c>
+      <c r="AD159" s="59"/>
+      <c r="AE159" s="59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:32" ht="18" x14ac:dyDescent="0.25">
+      <c r="A161" s="34" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="162" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A162" s="6"/>
+      <c r="B162" s="59"/>
+      <c r="C162" s="59">
+        <v>1</v>
+      </c>
+      <c r="D162" s="59"/>
+      <c r="E162" s="59"/>
+      <c r="F162" s="59">
+        <v>1</v>
+      </c>
+      <c r="G162" s="59"/>
+      <c r="H162" s="59">
+        <v>1</v>
+      </c>
+      <c r="I162" s="59"/>
+      <c r="J162" s="44">
+        <v>1</v>
+      </c>
+      <c r="K162" s="44"/>
+      <c r="L162" s="44"/>
+      <c r="M162" s="59"/>
+      <c r="N162" s="44"/>
+      <c r="O162" s="44">
+        <v>1</v>
+      </c>
+      <c r="P162" s="44"/>
+      <c r="Q162" s="59">
+        <v>1</v>
+      </c>
+      <c r="R162" s="43"/>
+      <c r="S162" s="43"/>
+      <c r="T162" s="45"/>
+      <c r="U162" s="45"/>
+      <c r="V162" s="45"/>
+      <c r="W162" s="43"/>
+      <c r="X162" s="45"/>
+      <c r="Y162" s="45"/>
+      <c r="Z162" s="45"/>
+      <c r="AA162" s="43">
+        <v>10</v>
+      </c>
+      <c r="AB162" s="37">
+        <v>1</v>
+      </c>
+      <c r="AC162" s="37">
+        <v>1</v>
+      </c>
+      <c r="AD162" s="37"/>
+      <c r="AE162" s="37"/>
+      <c r="AF162" s="37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164" spans="1:32" ht="18" x14ac:dyDescent="0.25">
+      <c r="A164" s="34" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="165" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A165" s="6"/>
+      <c r="B165" s="59">
+        <v>1</v>
+      </c>
+      <c r="C165" s="60"/>
+      <c r="D165" s="60"/>
+      <c r="E165" s="60"/>
+      <c r="F165" s="60"/>
+      <c r="G165" s="59">
+        <v>1</v>
+      </c>
+      <c r="H165" s="59">
+        <v>1</v>
+      </c>
+      <c r="I165" s="59"/>
+      <c r="J165" s="44">
+        <v>1</v>
+      </c>
+      <c r="K165" s="44">
+        <v>1</v>
+      </c>
+      <c r="L165" s="44"/>
+      <c r="M165" s="59">
+        <v>1</v>
+      </c>
+      <c r="N165" s="44">
+        <v>1</v>
+      </c>
+      <c r="O165" s="44">
+        <v>1</v>
+      </c>
+      <c r="P165" s="44"/>
+      <c r="Q165" s="59">
+        <v>1</v>
+      </c>
+      <c r="R165" s="59"/>
+      <c r="S165" s="59">
+        <v>1</v>
+      </c>
+      <c r="T165" s="44">
+        <v>1</v>
+      </c>
+      <c r="U165" s="44">
+        <v>1</v>
+      </c>
+      <c r="V165" s="44"/>
+      <c r="W165" s="59">
+        <v>1</v>
+      </c>
+      <c r="X165" s="44"/>
+      <c r="Y165" s="44">
+        <v>1</v>
+      </c>
+      <c r="Z165" s="44"/>
+      <c r="AA165" s="59"/>
+      <c r="AB165" s="37">
+        <v>1</v>
+      </c>
+      <c r="AC165" s="37"/>
+      <c r="AD165" s="37"/>
+      <c r="AE165" s="37">
+        <v>1</v>
+      </c>
+      <c r="AF165" s="66"/>
+    </row>
+    <row r="167" spans="1:32" ht="18" x14ac:dyDescent="0.25">
+      <c r="A167" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="S167" s="26"/>
+      <c r="U167" s="26"/>
+      <c r="V167" s="26"/>
+      <c r="W167" s="5">
+        <v>28</v>
+      </c>
+      <c r="X167" s="5">
+        <v>35</v>
+      </c>
+      <c r="Y167" s="5">
+        <v>59</v>
+      </c>
+      <c r="Z167" s="5">
+        <v>49</v>
+      </c>
+      <c r="AA167" s="5">
+        <v>55</v>
+      </c>
+      <c r="AB167" s="5">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="168" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A168" s="24"/>
+      <c r="B168" s="60"/>
+      <c r="C168" s="60"/>
+      <c r="D168" s="60"/>
+      <c r="E168" s="59">
+        <v>1</v>
+      </c>
+      <c r="F168" s="59">
+        <v>1</v>
+      </c>
+      <c r="G168" s="59"/>
+      <c r="H168" s="59">
+        <v>1</v>
+      </c>
+      <c r="I168" s="59"/>
+      <c r="J168" s="59"/>
+      <c r="K168" s="59">
+        <v>1</v>
+      </c>
+      <c r="L168" s="60"/>
+      <c r="M168" s="60"/>
+      <c r="N168" s="60"/>
+      <c r="O168" s="60"/>
+      <c r="P168" s="59">
+        <v>1</v>
+      </c>
+      <c r="Q168" s="59"/>
+      <c r="R168" s="44"/>
+      <c r="S168" s="44"/>
+      <c r="T168" s="44">
+        <v>1</v>
+      </c>
+      <c r="U168" s="59">
+        <v>1</v>
+      </c>
+      <c r="V168" s="59"/>
+      <c r="W168" s="59"/>
+      <c r="X168" s="59">
+        <v>1</v>
+      </c>
+      <c r="Y168" s="59"/>
+      <c r="Z168" s="52">
+        <v>1</v>
+      </c>
+      <c r="AA168" s="52"/>
+      <c r="AB168" s="52"/>
+      <c r="AC168" s="52"/>
+      <c r="AD168" s="59"/>
+      <c r="AE168" s="59"/>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>